<commit_message>
membuat controller rekap perorang
</commit_message>
<xml_diff>
--- a/server/assets/DISTRIBUSI.xlsx
+++ b/server/assets/DISTRIBUSI.xlsx
@@ -379,10 +379,10 @@
     <t>UPTD Perbekalan Obat dan Alkes</t>
   </si>
   <si>
-    <t>Agustina Rahmawati, S.A.P</t>
-  </si>
-  <si>
-    <t>NIP. 19800830 200212 2 009</t>
+    <t>Ibu Tina edit LAGI</t>
+  </si>
+  <si>
+    <t>NIP.666 662222</t>
   </si>
   <si>
     <t>SURAT  TUGAS</t>

</xml_diff>

<commit_message>
memperbaiki input data di excel
</commit_message>
<xml_diff>
--- a/server/assets/DISTRIBUSI.xlsx
+++ b/server/assets/DISTRIBUSI.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B878998-93D6-4959-A673-7B9686661234}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED85CD4A-6CC6-4BE9-BE97-5664B9ECF7B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1164" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1355" uniqueCount="161">
   <si>
     <t>LAPORAN PERJALANAN DINAS DALAM DAERAH</t>
   </si>
@@ -270,9 +270,6 @@
     <t>PADA TANGGAL</t>
   </si>
   <si>
-    <t>NOMOR SPD</t>
-  </si>
-  <si>
     <t>I.</t>
   </si>
   <si>
@@ -496,6 +493,30 @@
   </si>
   <si>
     <t>NIP.19780703 200502 2 006</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -1698,8 +1719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X51"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H54" sqref="H54"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N48" sqref="N48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1880,9 +1901,8 @@
       <c r="E6" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="9" t="str">
-        <f>SURTUG!$G$9</f>
-        <v>NOMOR SURAT TUGAS</v>
+      <c r="F6" s="9" t="s">
+        <v>159</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
@@ -1899,9 +1919,8 @@
       <c r="Q6" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="R6" s="9" t="str">
-        <f>SURTUG!$G$9</f>
-        <v>NOMOR SURAT TUGAS</v>
+      <c r="R6" s="9" t="s">
+        <v>159</v>
       </c>
       <c r="S6" s="9"/>
       <c r="T6" s="9"/>
@@ -1920,9 +1939,8 @@
       <c r="E7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="9" t="str">
-        <f>SURTUG!$G$12</f>
-        <v>TANGGAL BERANGKAT</v>
+      <c r="F7" s="9" t="s">
+        <v>159</v>
       </c>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
@@ -1939,9 +1957,8 @@
       <c r="Q7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="R7" s="9" t="str">
-        <f>SURTUG!$G$12</f>
-        <v>TANGGAL BERANGKAT</v>
+      <c r="R7" s="9" t="s">
+        <v>159</v>
       </c>
       <c r="S7" s="9"/>
       <c r="T7" s="9"/>
@@ -2024,9 +2041,8 @@
       <c r="G10" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H10" s="9" t="str">
-        <f>SURTUG!$G$16</f>
-        <v>NAMA1</v>
+      <c r="H10" s="9" t="s">
+        <v>159</v>
       </c>
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
@@ -2045,9 +2061,8 @@
       <c r="S10" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="T10" s="9" t="str">
-        <f>SURTUG!$G$16</f>
-        <v>NAMA1</v>
+      <c r="T10" s="9" t="s">
+        <v>159</v>
       </c>
       <c r="U10" s="9"/>
       <c r="V10" s="9"/>
@@ -2066,9 +2081,8 @@
       <c r="G11" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="9" t="str">
-        <f>SURTUG!$G$18</f>
-        <v>NIP1</v>
+      <c r="H11" s="9" t="s">
+        <v>159</v>
       </c>
       <c r="I11" s="9"/>
       <c r="J11" s="9"/>
@@ -2085,9 +2099,8 @@
       <c r="S11" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="T11" s="9" t="str">
-        <f>SURTUG!$G$18</f>
-        <v>NIP1</v>
+      <c r="T11" s="9" t="s">
+        <v>159</v>
       </c>
       <c r="U11" s="9"/>
       <c r="V11" s="9"/>
@@ -2134,9 +2147,8 @@
       <c r="G13" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H13" s="9" t="str">
-        <f>SURTUG!$G$21</f>
-        <v>NAMA2</v>
+      <c r="H13" s="9" t="s">
+        <v>159</v>
       </c>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
@@ -2155,9 +2167,8 @@
       <c r="S13" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="T13" s="9" t="str">
-        <f>SURTUG!$G$21</f>
-        <v>NAMA2</v>
+      <c r="T13" s="9" t="s">
+        <v>159</v>
       </c>
       <c r="U13" s="9"/>
       <c r="V13" s="9"/>
@@ -2176,9 +2187,8 @@
       <c r="G14" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H14" s="9" t="str">
-        <f>SURTUG!$G$23</f>
-        <v>NIP2</v>
+      <c r="H14" s="9" t="s">
+        <v>159</v>
       </c>
       <c r="I14" s="9"/>
       <c r="J14" s="9"/>
@@ -2195,9 +2205,8 @@
       <c r="S14" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="T14" s="9" t="str">
-        <f>SURTUG!$G$23</f>
-        <v>NIP2</v>
+      <c r="T14" s="9" t="s">
+        <v>159</v>
       </c>
       <c r="U14" s="9"/>
       <c r="V14" s="9"/>
@@ -2244,9 +2253,8 @@
       <c r="G16" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H16" s="9" t="str">
-        <f>SURTUG!$G$26</f>
-        <v>NAMA3</v>
+      <c r="H16" s="9" t="s">
+        <v>159</v>
       </c>
       <c r="I16" s="9"/>
       <c r="J16" s="9"/>
@@ -2265,9 +2273,8 @@
       <c r="S16" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="T16" s="9" t="str">
-        <f>SURTUG!$G$26</f>
-        <v>NAMA3</v>
+      <c r="T16" s="9" t="s">
+        <v>159</v>
       </c>
       <c r="U16" s="9"/>
       <c r="V16" s="9"/>
@@ -2286,9 +2293,8 @@
       <c r="G17" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H17" s="9" t="str">
-        <f>SURTUG!$G$28</f>
-        <v>NIP3</v>
+      <c r="H17" s="9" t="s">
+        <v>159</v>
       </c>
       <c r="I17" s="9"/>
       <c r="J17" s="9"/>
@@ -2305,9 +2311,8 @@
       <c r="S17" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="T17" s="9" t="str">
-        <f>SURTUG!$G$28</f>
-        <v>NIP3</v>
+      <c r="T17" s="9" t="s">
+        <v>159</v>
       </c>
       <c r="U17" s="9"/>
       <c r="V17" s="9"/>
@@ -2384,9 +2389,8 @@
       <c r="E20" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F20" s="9" t="str">
-        <f>SURTUG!$G$38</f>
-        <v>NAMA PUSKESMAS</v>
+      <c r="F20" s="9" t="s">
+        <v>159</v>
       </c>
       <c r="G20" s="9"/>
       <c r="H20" s="9"/>
@@ -2403,9 +2407,8 @@
       <c r="Q20" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="R20" s="9" t="str">
-        <f>SURTUG!$G$38</f>
-        <v>NAMA PUSKESMAS</v>
+      <c r="R20" s="9" t="s">
+        <v>159</v>
       </c>
       <c r="S20" s="9"/>
       <c r="T20" s="9"/>
@@ -2424,9 +2427,8 @@
       <c r="E21" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F21" s="9" t="str">
-        <f>SURTUG!$G$12</f>
-        <v>TANGGAL BERANGKAT</v>
+      <c r="F21" s="9" t="s">
+        <v>159</v>
       </c>
       <c r="G21" s="9"/>
       <c r="H21" s="9"/>
@@ -2443,9 +2445,8 @@
       <c r="Q21" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="R21" s="9" t="str">
-        <f>SURTUG!$G$12</f>
-        <v>TANGGAL BERANGKAT</v>
+      <c r="R21" s="9" t="s">
+        <v>159</v>
       </c>
       <c r="S21" s="9"/>
       <c r="T21" s="9"/>
@@ -3034,9 +3035,8 @@
       <c r="G41" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H41" s="9" t="str">
-        <f>SURTUG!$G$16</f>
-        <v>NAMA1</v>
+      <c r="H41" s="9" t="s">
+        <v>159</v>
       </c>
       <c r="I41" s="9"/>
       <c r="J41" s="9"/>
@@ -3053,9 +3053,8 @@
       <c r="S41" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="T41" s="9" t="str">
-        <f>SURTUG!$G$16</f>
-        <v>NAMA1</v>
+      <c r="T41" s="9" t="s">
+        <v>159</v>
       </c>
       <c r="U41" s="9"/>
       <c r="V41" s="9"/>
@@ -3100,9 +3099,8 @@
       <c r="G43" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="H43" s="9" t="str">
-        <f>SURTUG!$G$21</f>
-        <v>NAMA2</v>
+      <c r="H43" s="9" t="s">
+        <v>159</v>
       </c>
       <c r="I43" s="9"/>
       <c r="J43" s="9"/>
@@ -3119,9 +3117,8 @@
       <c r="S43" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="T43" s="9" t="str">
-        <f>SURTUG!$G$21</f>
-        <v>NAMA2</v>
+      <c r="T43" s="9" t="s">
+        <v>159</v>
       </c>
       <c r="U43" s="9"/>
       <c r="V43" s="9"/>
@@ -3132,9 +3129,8 @@
     </row>
     <row r="44" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A44" s="9"/>
-      <c r="B44" s="10" t="str">
-        <f>SURTUG!$G$50</f>
-        <v>Yayillatul Rochmah, S. Si. Apt</v>
+      <c r="B44" s="10" t="s">
+        <v>160</v>
       </c>
       <c r="C44" s="10"/>
       <c r="D44" s="10"/>
@@ -3147,9 +3143,8 @@
       <c r="K44" s="8"/>
       <c r="L44" s="9"/>
       <c r="M44" s="9"/>
-      <c r="N44" s="10" t="str">
-        <f>SURTUG!$G$50</f>
-        <v>Yayillatul Rochmah, S. Si. Apt</v>
+      <c r="N44" s="10" t="s">
+        <v>160</v>
       </c>
       <c r="O44" s="10"/>
       <c r="P44" s="10"/>
@@ -3164,9 +3159,8 @@
     </row>
     <row r="45" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A45" s="9"/>
-      <c r="B45" s="11" t="str">
-        <f>SURTUG!$G$51</f>
-        <v>NIP.19780703 200502 2 006</v>
+      <c r="B45" s="11" t="s">
+        <v>160</v>
       </c>
       <c r="C45" s="11"/>
       <c r="D45" s="11"/>
@@ -3175,9 +3169,8 @@
       <c r="G45" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H45" s="9" t="str">
-        <f>SURTUG!$G$26</f>
-        <v>NAMA3</v>
+      <c r="H45" s="9" t="s">
+        <v>159</v>
       </c>
       <c r="I45" s="9"/>
       <c r="J45" s="9"/>
@@ -3186,9 +3179,8 @@
       </c>
       <c r="L45" s="9"/>
       <c r="M45" s="9"/>
-      <c r="N45" s="11" t="str">
-        <f>SURTUG!$G$51</f>
-        <v>NIP.19780703 200502 2 006</v>
+      <c r="N45" s="11" t="s">
+        <v>160</v>
       </c>
       <c r="O45" s="11"/>
       <c r="P45" s="11"/>
@@ -3197,9 +3189,8 @@
       <c r="S45" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="T45" s="9" t="str">
-        <f>SURTUG!$G$26</f>
-        <v>NAMA3</v>
+      <c r="T45" s="9" t="s">
+        <v>159</v>
       </c>
       <c r="U45" s="9"/>
       <c r="V45" s="9"/>
@@ -3372,7 +3363,7 @@
     <mergeCell ref="R28:X32"/>
   </mergeCells>
   <pageMargins left="0.57291666666666663" right="0.51041666666666663" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="5" orientation="portrait" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="5" orientation="portrait" useFirstPageNumber="1" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3380,8 +3371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:V45"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19:K20"/>
+    <sheetView view="pageLayout" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P45" sqref="P45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3575,9 +3566,8 @@
       <c r="G9" t="s">
         <v>6</v>
       </c>
-      <c r="H9" t="str">
-        <f>SPD!H9</f>
-        <v>NOMOR SPD</v>
+      <c r="H9" t="s">
+        <v>158</v>
       </c>
       <c r="Q9" t="s">
         <v>42</v>
@@ -3585,9 +3575,8 @@
       <c r="R9" t="s">
         <v>6</v>
       </c>
-      <c r="S9" t="str">
-        <f>H9</f>
-        <v>NOMOR SPD</v>
+      <c r="S9" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:22" ht="9.1999999999999993" customHeight="1" x14ac:dyDescent="0.25">
@@ -3745,9 +3734,8 @@
       <c r="D15" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="20" t="str">
-        <f>SURTUG!G26</f>
-        <v>NAMA3</v>
+      <c r="E15" s="20" t="s">
+        <v>158</v>
       </c>
       <c r="F15" s="19"/>
       <c r="G15" s="19"/>
@@ -3765,9 +3753,8 @@
       <c r="O15" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="P15" s="20" t="str">
-        <f>E15</f>
-        <v>NAMA3</v>
+      <c r="P15" s="20" t="s">
+        <v>158</v>
       </c>
       <c r="Q15" s="19"/>
       <c r="R15" s="19"/>
@@ -3790,9 +3777,8 @@
       <c r="E16" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="F16" s="21" t="str">
-        <f>SURTUG!G27</f>
-        <v>PANGKAT3</v>
+      <c r="F16" s="21" t="s">
+        <v>158</v>
       </c>
       <c r="G16" s="21"/>
       <c r="H16" s="21"/>
@@ -3812,9 +3798,8 @@
       <c r="P16" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="Q16" s="21" t="str">
-        <f>F16</f>
-        <v>PANGKAT3</v>
+      <c r="Q16" s="21" t="s">
+        <v>158</v>
       </c>
       <c r="R16" s="21"/>
       <c r="S16" s="21"/>
@@ -3834,9 +3819,8 @@
       <c r="E17" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="F17" s="21" t="str">
-        <f>SURTUG!G29</f>
-        <v>JABATAN3</v>
+      <c r="F17" s="21" t="s">
+        <v>158</v>
       </c>
       <c r="G17" s="21"/>
       <c r="H17" s="21"/>
@@ -3854,9 +3838,8 @@
       <c r="P17" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="Q17" s="21" t="str">
-        <f>F17</f>
-        <v>JABATAN3</v>
+      <c r="Q17" s="21" t="s">
+        <v>158</v>
       </c>
       <c r="R17" s="21"/>
       <c r="S17" s="21"/>
@@ -4071,9 +4054,8 @@
       <c r="O23" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="P23" s="19" t="str">
-        <f>SURTUG!R38</f>
-        <v>NAMA PUSKESMAS</v>
+      <c r="P23" s="19" t="s">
+        <v>158</v>
       </c>
       <c r="Q23" s="19"/>
       <c r="R23" s="19"/>
@@ -4133,9 +4115,8 @@
       <c r="D25" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E25" s="21" t="str">
-        <f>SURTUG!$G$32</f>
-        <v>TANGGAL BERANGKAT</v>
+      <c r="E25" s="21" t="s">
+        <v>158</v>
       </c>
       <c r="F25" s="21"/>
       <c r="G25" s="21"/>
@@ -4151,9 +4132,8 @@
       <c r="O25" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="P25" s="21" t="str">
-        <f>SURTUG!R32</f>
-        <v>TANGGAL BERANGKAT</v>
+      <c r="P25" s="21" t="s">
+        <v>158</v>
       </c>
       <c r="Q25" s="21"/>
       <c r="R25" s="21"/>
@@ -4171,9 +4151,8 @@
       <c r="D26" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E26" s="19" t="str">
-        <f>SURTUG!$G$33</f>
-        <v>TANGGAL PULANG</v>
+      <c r="E26" s="19" t="s">
+        <v>158</v>
       </c>
       <c r="F26" s="19"/>
       <c r="G26" s="19"/>
@@ -4189,9 +4168,8 @@
       <c r="O26" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="P26" s="19" t="str">
-        <f>SURTUG!R33</f>
-        <v>TANGGAL PULANG</v>
+      <c r="P26" s="19" t="s">
+        <v>158</v>
       </c>
       <c r="Q26" s="19"/>
       <c r="R26" s="19"/>
@@ -4457,9 +4435,8 @@
       <c r="G34" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="H34" s="26" t="str">
-        <f>SURTUG!$G$32</f>
-        <v>TANGGAL BERANGKAT</v>
+      <c r="H34" s="26" t="s">
+        <v>158</v>
       </c>
       <c r="I34" s="26"/>
       <c r="J34" s="9"/>
@@ -4474,9 +4451,8 @@
       <c r="R34" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="S34" s="26" t="str">
-        <f>SURTUG!R32</f>
-        <v>TANGGAL BERANGKAT</v>
+      <c r="S34" s="26" t="s">
+        <v>158</v>
       </c>
       <c r="T34" s="26"/>
       <c r="U34" s="9"/>
@@ -4611,9 +4587,8 @@
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
-      <c r="E40" s="27" t="str">
-        <f>SURTUG!$G$50</f>
-        <v>Yayillatul Rochmah, S. Si. Apt</v>
+      <c r="E40" s="27" t="s">
+        <v>160</v>
       </c>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
@@ -4625,9 +4600,8 @@
       <c r="M40" s="7"/>
       <c r="N40" s="7"/>
       <c r="O40" s="7"/>
-      <c r="P40" s="27" t="str">
-        <f>SURTUG!R50</f>
-        <v>Yayillatul Rochmah, S. Si. Apt</v>
+      <c r="P40" s="27" t="s">
+        <v>160</v>
       </c>
       <c r="Q40" s="6"/>
       <c r="R40" s="6"/>
@@ -4641,9 +4615,8 @@
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
-      <c r="E41" s="6" t="str">
-        <f>SURTUG!$G$51</f>
-        <v>NIP.19780703 200502 2 006</v>
+      <c r="E41" s="6" t="s">
+        <v>160</v>
       </c>
       <c r="F41" s="6"/>
       <c r="G41" s="6"/>
@@ -4655,9 +4628,8 @@
       <c r="M41" s="7"/>
       <c r="N41" s="7"/>
       <c r="O41" s="7"/>
-      <c r="P41" s="6" t="str">
-        <f>SURTUG!R51</f>
-        <v>NIP.19780703 200502 2 006</v>
+      <c r="P41" s="6" t="s">
+        <v>160</v>
       </c>
       <c r="Q41" s="6"/>
       <c r="R41" s="6"/>
@@ -4768,7 +4740,7 @@
     <mergeCell ref="P19:V20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.3125" bottom="0.28409090909090912" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="5" orientation="portrait" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="5" orientation="portrait" useFirstPageNumber="1" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -4777,8 +4749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:V45"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView view="pageLayout" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P44" sqref="P44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4972,9 +4944,8 @@
       <c r="G9" t="s">
         <v>6</v>
       </c>
-      <c r="H9" t="str">
-        <f>SPD!H9</f>
-        <v>NOMOR SPD</v>
+      <c r="H9" t="s">
+        <v>157</v>
       </c>
       <c r="Q9" t="s">
         <v>42</v>
@@ -4982,9 +4953,8 @@
       <c r="R9" t="s">
         <v>6</v>
       </c>
-      <c r="S9" t="str">
-        <f>H9</f>
-        <v>NOMOR SPD</v>
+      <c r="S9" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:22" ht="9.1999999999999993" customHeight="1" x14ac:dyDescent="0.25">
@@ -5142,9 +5112,8 @@
       <c r="D15" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="20" t="str">
-        <f>SURTUG!G21</f>
-        <v>NAMA2</v>
+      <c r="E15" s="20" t="s">
+        <v>157</v>
       </c>
       <c r="F15" s="19"/>
       <c r="G15" s="19"/>
@@ -5164,7 +5133,7 @@
       </c>
       <c r="P15" s="20" t="str">
         <f>E15</f>
-        <v>NAMA2</v>
+        <v>r</v>
       </c>
       <c r="Q15" s="19"/>
       <c r="R15" s="19"/>
@@ -5187,9 +5156,8 @@
       <c r="E16" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="F16" s="21" t="str">
-        <f>SURTUG!G22</f>
-        <v>PANGKAT2</v>
+      <c r="F16" s="21" t="s">
+        <v>157</v>
       </c>
       <c r="G16" s="21"/>
       <c r="H16" s="21"/>
@@ -5209,9 +5177,8 @@
       <c r="P16" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="Q16" s="21" t="str">
-        <f>F16</f>
-        <v>PANGKAT2</v>
+      <c r="Q16" s="21" t="s">
+        <v>157</v>
       </c>
       <c r="R16" s="21"/>
       <c r="S16" s="21"/>
@@ -5231,9 +5198,8 @@
       <c r="E17" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="F17" s="21" t="str">
-        <f>SURTUG!G24</f>
-        <v>JABATAN2</v>
+      <c r="F17" s="21" t="s">
+        <v>157</v>
       </c>
       <c r="G17" s="21"/>
       <c r="H17" s="21"/>
@@ -5251,9 +5217,8 @@
       <c r="P17" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="Q17" s="21" t="str">
-        <f>F17</f>
-        <v>JABATAN2</v>
+      <c r="Q17" s="21" t="s">
+        <v>157</v>
       </c>
       <c r="R17" s="21"/>
       <c r="S17" s="21"/>
@@ -5450,9 +5415,8 @@
       <c r="D23" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E23" s="19" t="str">
-        <f>SURTUG!$G$38</f>
-        <v>NAMA PUSKESMAS</v>
+      <c r="E23" s="19" t="s">
+        <v>157</v>
       </c>
       <c r="F23" s="19"/>
       <c r="G23" s="19"/>
@@ -5468,9 +5432,8 @@
       <c r="O23" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="P23" s="19" t="str">
-        <f>SURTUG!R38</f>
-        <v>NAMA PUSKESMAS</v>
+      <c r="P23" s="19" t="s">
+        <v>157</v>
       </c>
       <c r="Q23" s="19"/>
       <c r="R23" s="19"/>
@@ -5530,9 +5493,8 @@
       <c r="D25" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E25" s="21" t="str">
-        <f>SURTUG!$G$32</f>
-        <v>TANGGAL BERANGKAT</v>
+      <c r="E25" s="21" t="s">
+        <v>157</v>
       </c>
       <c r="F25" s="21"/>
       <c r="G25" s="21"/>
@@ -5548,9 +5510,8 @@
       <c r="O25" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="P25" s="21" t="str">
-        <f>SURTUG!R32</f>
-        <v>TANGGAL BERANGKAT</v>
+      <c r="P25" s="21" t="s">
+        <v>157</v>
       </c>
       <c r="Q25" s="21"/>
       <c r="R25" s="21"/>
@@ -5568,9 +5529,8 @@
       <c r="D26" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E26" s="19" t="str">
-        <f>SURTUG!$G$33</f>
-        <v>TANGGAL PULANG</v>
+      <c r="E26" s="19" t="s">
+        <v>157</v>
       </c>
       <c r="F26" s="19"/>
       <c r="G26" s="19"/>
@@ -5586,9 +5546,8 @@
       <c r="O26" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="P26" s="19" t="str">
-        <f>SURTUG!R33</f>
-        <v>TANGGAL PULANG</v>
+      <c r="P26" s="19" t="s">
+        <v>157</v>
       </c>
       <c r="Q26" s="19"/>
       <c r="R26" s="19"/>
@@ -5854,9 +5813,8 @@
       <c r="G34" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="H34" s="26" t="str">
-        <f>SURTUG!$G$32</f>
-        <v>TANGGAL BERANGKAT</v>
+      <c r="H34" s="26" t="s">
+        <v>157</v>
       </c>
       <c r="I34" s="26"/>
       <c r="J34" s="9"/>
@@ -5871,9 +5829,8 @@
       <c r="R34" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="S34" s="26" t="str">
-        <f>SURTUG!R32</f>
-        <v>TANGGAL BERANGKAT</v>
+      <c r="S34" s="26" t="s">
+        <v>157</v>
       </c>
       <c r="T34" s="26"/>
       <c r="U34" s="9"/>
@@ -6008,9 +5965,8 @@
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
-      <c r="E40" s="27" t="str">
-        <f>SURTUG!$G$50</f>
-        <v>Yayillatul Rochmah, S. Si. Apt</v>
+      <c r="E40" s="27" t="s">
+        <v>160</v>
       </c>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
@@ -6022,9 +5978,8 @@
       <c r="M40" s="7"/>
       <c r="N40" s="7"/>
       <c r="O40" s="7"/>
-      <c r="P40" s="27" t="str">
-        <f>SURTUG!R50</f>
-        <v>Yayillatul Rochmah, S. Si. Apt</v>
+      <c r="P40" s="27" t="s">
+        <v>160</v>
       </c>
       <c r="Q40" s="6"/>
       <c r="R40" s="6"/>
@@ -6038,9 +5993,8 @@
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
-      <c r="E41" s="6" t="str">
-        <f>SURTUG!$G$51</f>
-        <v>NIP.19780703 200502 2 006</v>
+      <c r="E41" s="6" t="s">
+        <v>160</v>
       </c>
       <c r="F41" s="6"/>
       <c r="G41" s="6"/>
@@ -6052,9 +6006,8 @@
       <c r="M41" s="7"/>
       <c r="N41" s="7"/>
       <c r="O41" s="7"/>
-      <c r="P41" s="6" t="str">
-        <f>SURTUG!R51</f>
-        <v>NIP.19780703 200502 2 006</v>
+      <c r="P41" s="6" t="s">
+        <v>160</v>
       </c>
       <c r="Q41" s="6"/>
       <c r="R41" s="6"/>
@@ -6165,7 +6118,7 @@
     <mergeCell ref="P19:V20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.3125" bottom="0.28409090909090912" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="5" orientation="portrait" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="5" orientation="portrait" useFirstPageNumber="1" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -6174,8 +6127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:V45"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19:K20"/>
+    <sheetView view="pageLayout" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P44" sqref="P44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6370,7 +6323,7 @@
         <v>6</v>
       </c>
       <c r="H9" t="s">
-        <v>78</v>
+        <v>156</v>
       </c>
       <c r="Q9" t="s">
         <v>42</v>
@@ -6378,9 +6331,8 @@
       <c r="R9" t="s">
         <v>6</v>
       </c>
-      <c r="S9" t="str">
-        <f>H9</f>
-        <v>NOMOR SPD</v>
+      <c r="S9" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="10" spans="1:22" ht="9.1999999999999993" customHeight="1" x14ac:dyDescent="0.25">
@@ -6538,9 +6490,8 @@
       <c r="D15" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="20" t="str">
-        <f>SURTUG!G16</f>
-        <v>NAMA1</v>
+      <c r="E15" s="20" t="s">
+        <v>156</v>
       </c>
       <c r="F15" s="19"/>
       <c r="G15" s="19"/>
@@ -6558,9 +6509,8 @@
       <c r="O15" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="P15" s="20" t="str">
-        <f>SURTUG!R16</f>
-        <v>NAMA1</v>
+      <c r="P15" s="20" t="s">
+        <v>156</v>
       </c>
       <c r="Q15" s="19"/>
       <c r="R15" s="19"/>
@@ -6583,9 +6533,8 @@
       <c r="E16" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="F16" s="21" t="str">
-        <f>SURTUG!G17</f>
-        <v>PANGKAT1</v>
+      <c r="F16" s="21" t="s">
+        <v>156</v>
       </c>
       <c r="G16" s="21"/>
       <c r="H16" s="21"/>
@@ -6605,9 +6554,8 @@
       <c r="P16" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="Q16" s="21" t="str">
-        <f>SURTUG!R17</f>
-        <v>PANGKAT1</v>
+      <c r="Q16" s="21" t="s">
+        <v>156</v>
       </c>
       <c r="R16" s="21"/>
       <c r="S16" s="21"/>
@@ -6627,9 +6575,8 @@
       <c r="E17" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="F17" s="21" t="str">
-        <f>SURTUG!G19</f>
-        <v>JABATAN1</v>
+      <c r="F17" s="21" t="s">
+        <v>156</v>
       </c>
       <c r="G17" s="21"/>
       <c r="H17" s="21"/>
@@ -6647,9 +6594,8 @@
       <c r="P17" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="Q17" s="21" t="str">
-        <f>SURTUG!R19</f>
-        <v>JABATAN1</v>
+      <c r="Q17" s="21" t="s">
+        <v>156</v>
       </c>
       <c r="R17" s="21"/>
       <c r="S17" s="21"/>
@@ -6846,9 +6792,8 @@
       <c r="D23" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E23" s="19" t="str">
-        <f>SURTUG!$G$38</f>
-        <v>NAMA PUSKESMAS</v>
+      <c r="E23" s="19" t="s">
+        <v>156</v>
       </c>
       <c r="F23" s="19"/>
       <c r="G23" s="19"/>
@@ -6864,9 +6809,8 @@
       <c r="O23" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="P23" s="19" t="str">
-        <f>SURTUG!R38</f>
-        <v>NAMA PUSKESMAS</v>
+      <c r="P23" s="19" t="s">
+        <v>156</v>
       </c>
       <c r="Q23" s="19"/>
       <c r="R23" s="19"/>
@@ -6926,9 +6870,8 @@
       <c r="D25" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E25" s="21" t="str">
-        <f>SURTUG!$G$32</f>
-        <v>TANGGAL BERANGKAT</v>
+      <c r="E25" s="21" t="s">
+        <v>156</v>
       </c>
       <c r="F25" s="21"/>
       <c r="G25" s="21"/>
@@ -6944,9 +6887,8 @@
       <c r="O25" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="P25" s="21" t="str">
-        <f>SURTUG!R32</f>
-        <v>TANGGAL BERANGKAT</v>
+      <c r="P25" s="21" t="s">
+        <v>156</v>
       </c>
       <c r="Q25" s="21"/>
       <c r="R25" s="21"/>
@@ -6964,9 +6906,8 @@
       <c r="D26" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E26" s="19" t="str">
-        <f>SURTUG!$G$33</f>
-        <v>TANGGAL PULANG</v>
+      <c r="E26" s="19" t="s">
+        <v>156</v>
       </c>
       <c r="F26" s="19"/>
       <c r="G26" s="19"/>
@@ -6982,9 +6923,8 @@
       <c r="O26" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="P26" s="19" t="str">
-        <f>SURTUG!R33</f>
-        <v>TANGGAL PULANG</v>
+      <c r="P26" s="19" t="s">
+        <v>156</v>
       </c>
       <c r="Q26" s="19"/>
       <c r="R26" s="19"/>
@@ -7250,9 +7190,8 @@
       <c r="G34" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="H34" s="26" t="str">
-        <f>SURTUG!$G$32</f>
-        <v>TANGGAL BERANGKAT</v>
+      <c r="H34" s="26" t="s">
+        <v>156</v>
       </c>
       <c r="I34" s="26"/>
       <c r="J34" s="9"/>
@@ -7267,9 +7206,8 @@
       <c r="R34" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="S34" s="26" t="str">
-        <f>SURTUG!R32</f>
-        <v>TANGGAL BERANGKAT</v>
+      <c r="S34" s="26" t="s">
+        <v>156</v>
       </c>
       <c r="T34" s="26"/>
       <c r="U34" s="9"/>
@@ -7404,9 +7342,8 @@
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
-      <c r="E40" s="27" t="str">
-        <f>SURTUG!$G$50</f>
-        <v>Yayillatul Rochmah, S. Si. Apt</v>
+      <c r="E40" s="27" t="s">
+        <v>160</v>
       </c>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
@@ -7418,9 +7355,8 @@
       <c r="M40" s="7"/>
       <c r="N40" s="7"/>
       <c r="O40" s="7"/>
-      <c r="P40" s="27" t="str">
-        <f>SURTUG!R50</f>
-        <v>Yayillatul Rochmah, S. Si. Apt</v>
+      <c r="P40" s="27" t="s">
+        <v>160</v>
       </c>
       <c r="Q40" s="6"/>
       <c r="R40" s="6"/>
@@ -7434,9 +7370,8 @@
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
-      <c r="E41" s="6" t="str">
-        <f>SURTUG!$G$51</f>
-        <v>NIP.19780703 200502 2 006</v>
+      <c r="E41" s="6" t="s">
+        <v>160</v>
       </c>
       <c r="F41" s="6"/>
       <c r="G41" s="6"/>
@@ -7448,9 +7383,8 @@
       <c r="M41" s="7"/>
       <c r="N41" s="7"/>
       <c r="O41" s="7"/>
-      <c r="P41" s="6" t="str">
-        <f>SURTUG!R51</f>
-        <v>NIP.19780703 200502 2 006</v>
+      <c r="P41" s="6" t="s">
+        <v>160</v>
       </c>
       <c r="Q41" s="6"/>
       <c r="R41" s="6"/>
@@ -7561,7 +7495,7 @@
     <mergeCell ref="P19:V20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.3125" bottom="0.28409090909090912" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="5" orientation="portrait" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="5" orientation="portrait" useFirstPageNumber="1" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -7570,8 +7504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AM82"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+    <sheetView view="pageLayout" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AE85" sqref="AE85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="19.7" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7619,60 +7553,57 @@
     <row r="1" spans="1:39" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E1" s="28"/>
       <c r="F1" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="G1" s="7" t="s">
-        <v>80</v>
-      </c>
       <c r="H1" s="7" t="s">
         <v>6</v>
       </c>
       <c r="L1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="9" t="str">
-        <f>SPD!H9</f>
-        <v>NOMOR SPD</v>
+      <c r="M1" s="9" t="s">
+        <v>155</v>
       </c>
       <c r="R1" s="28"/>
       <c r="S1" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="T1" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="T1" s="7" t="s">
-        <v>80</v>
-      </c>
       <c r="U1" s="7" t="s">
         <v>6</v>
       </c>
       <c r="Y1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="Z1" s="9" t="str">
-        <f>M1</f>
-        <v>NOMOR SPD</v>
+      <c r="Z1" s="9" t="s">
+        <v>155</v>
       </c>
       <c r="AE1" s="28"/>
       <c r="AF1" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="AG1" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="AG1" s="7" t="s">
-        <v>80</v>
-      </c>
       <c r="AH1" s="7" t="s">
         <v>6</v>
       </c>
       <c r="AL1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="AM1" s="9" t="str">
-        <f>M1</f>
-        <v>NOMOR SPD</v>
+      <c r="AM1" s="9" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:39" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E2" s="28"/>
       <c r="G2" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>6</v>
@@ -7688,7 +7619,7 @@
       </c>
       <c r="R2" s="28"/>
       <c r="T2" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="U2" s="7" t="s">
         <v>6</v>
@@ -7704,7 +7635,7 @@
       </c>
       <c r="AE2" s="28"/>
       <c r="AG2" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AH2" s="7" t="s">
         <v>6</v>
@@ -7722,21 +7653,21 @@
     <row r="3" spans="1:39" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E3" s="28"/>
       <c r="G3" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="R3" s="28"/>
       <c r="T3" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AE3" s="28"/>
       <c r="AG3" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:39" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E4" s="28"/>
       <c r="G4" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>6</v>
@@ -7744,13 +7675,12 @@
       <c r="L4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="M4" s="7" t="str">
-        <f>SURTUG!$G$32</f>
-        <v>TANGGAL BERANGKAT</v>
+      <c r="M4" s="7" t="s">
+        <v>155</v>
       </c>
       <c r="R4" s="28"/>
       <c r="T4" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="U4" s="7" t="s">
         <v>6</v>
@@ -7758,13 +7688,12 @@
       <c r="Y4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="Z4" s="7" t="str">
-        <f>SURTUG!$G$32</f>
-        <v>TANGGAL BERANGKAT</v>
+      <c r="Z4" s="7" t="s">
+        <v>155</v>
       </c>
       <c r="AE4" s="28"/>
       <c r="AG4" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AH4" s="7" t="s">
         <v>6</v>
@@ -7772,15 +7701,14 @@
       <c r="AL4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="AM4" s="7" t="str">
-        <f>SURTUG!$G$32</f>
-        <v>TANGGAL BERANGKAT</v>
+      <c r="AM4" s="7" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:39" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E5" s="28"/>
       <c r="G5" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>6</v>
@@ -7788,13 +7716,12 @@
       <c r="L5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="M5" s="9" t="str">
-        <f>SURTUG!$G$38</f>
-        <v>NAMA PUSKESMAS</v>
+      <c r="M5" s="9" t="s">
+        <v>155</v>
       </c>
       <c r="R5" s="28"/>
       <c r="T5" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="U5" s="7" t="s">
         <v>6</v>
@@ -7802,13 +7729,12 @@
       <c r="Y5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="Z5" s="9" t="str">
-        <f>SURTUG!$G$38</f>
-        <v>NAMA PUSKESMAS</v>
+      <c r="Z5" s="9" t="s">
+        <v>155</v>
       </c>
       <c r="AE5" s="28"/>
       <c r="AG5" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AH5" s="7" t="s">
         <v>6</v>
@@ -7816,9 +7742,8 @@
       <c r="AL5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="AM5" s="9" t="str">
-        <f>SURTUG!$G$38</f>
-        <v>NAMA PUSKESMAS</v>
+      <c r="AM5" s="9" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:39" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -7874,21 +7799,20 @@
     </row>
     <row r="9" spans="1:39" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>86</v>
-      </c>
       <c r="C9" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="9" t="str">
-        <f>M5</f>
-        <v>NAMA PUSKESMAS</v>
+      <c r="D9" s="9" t="s">
+        <v>155</v>
       </c>
       <c r="E9" s="28"/>
       <c r="G9" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>6</v>
@@ -7896,26 +7820,24 @@
       <c r="L9" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="M9" s="9" t="str">
-        <f>D9</f>
-        <v>NAMA PUSKESMAS</v>
+      <c r="M9" s="9" t="s">
+        <v>155</v>
       </c>
       <c r="N9" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="O9" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="O9" s="7" t="s">
-        <v>86</v>
-      </c>
       <c r="P9" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="Q9" s="9" t="str">
-        <f>Z5</f>
-        <v>NAMA PUSKESMAS</v>
+      <c r="Q9" s="9" t="s">
+        <v>155</v>
       </c>
       <c r="R9" s="28"/>
       <c r="T9" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="U9" s="7" t="s">
         <v>6</v>
@@ -7923,26 +7845,24 @@
       <c r="Y9" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="Z9" s="9" t="str">
-        <f>Q9</f>
-        <v>NAMA PUSKESMAS</v>
+      <c r="Z9" s="9" t="s">
+        <v>155</v>
       </c>
       <c r="AA9" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB9" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="AB9" s="7" t="s">
-        <v>86</v>
-      </c>
       <c r="AC9" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="AD9" s="9" t="str">
-        <f>AM5</f>
-        <v>NAMA PUSKESMAS</v>
+      <c r="AD9" s="9" t="s">
+        <v>155</v>
       </c>
       <c r="AE9" s="28"/>
       <c r="AG9" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AH9" s="7" t="s">
         <v>6</v>
@@ -7950,25 +7870,23 @@
       <c r="AL9" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="AM9" s="9" t="str">
-        <f>AD9</f>
-        <v>NAMA PUSKESMAS</v>
+      <c r="AM9" s="9" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="10" spans="1:39" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="7" t="str">
-        <f>M4</f>
-        <v>TANGGAL BERANGKAT</v>
+      <c r="D10" s="7" t="s">
+        <v>155</v>
       </c>
       <c r="E10" s="28"/>
       <c r="G10" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H10" s="7" t="s">
         <v>6</v>
@@ -7981,18 +7899,17 @@
         <v>Tana Paser</v>
       </c>
       <c r="O10" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P10" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="Q10" s="7" t="str">
-        <f>Z4</f>
-        <v>TANGGAL BERANGKAT</v>
+      <c r="Q10" s="7" t="s">
+        <v>155</v>
       </c>
       <c r="R10" s="28"/>
       <c r="T10" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="U10" s="7" t="s">
         <v>6</v>
@@ -8005,18 +7922,17 @@
         <v>Tana Paser</v>
       </c>
       <c r="AB10" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AC10" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="AD10" s="7" t="str">
-        <f>AM4</f>
-        <v>TANGGAL BERANGKAT</v>
+      <c r="AD10" s="7" t="s">
+        <v>155</v>
       </c>
       <c r="AE10" s="28"/>
       <c r="AG10" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AH10" s="7" t="s">
         <v>6</v>
@@ -8031,14 +7947,14 @@
     </row>
     <row r="11" spans="1:39" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E11" s="28"/>
       <c r="G11" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H11" s="7" t="s">
         <v>6</v>
@@ -8046,19 +7962,18 @@
       <c r="L11" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="M11" s="7" t="str">
-        <f>SURTUG!$G$33</f>
-        <v>TANGGAL PULANG</v>
+      <c r="M11" s="7" t="s">
+        <v>155</v>
       </c>
       <c r="O11" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P11" s="7" t="s">
         <v>6</v>
       </c>
       <c r="R11" s="28"/>
       <c r="T11" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="U11" s="7" t="s">
         <v>6</v>
@@ -8066,19 +7981,18 @@
       <c r="Y11" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="Z11" s="7" t="str">
-        <f>SURTUG!$G$33</f>
-        <v>TANGGAL PULANG</v>
+      <c r="Z11" s="7" t="s">
+        <v>155</v>
       </c>
       <c r="AB11" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AC11" s="7" t="s">
         <v>6</v>
       </c>
       <c r="AE11" s="28"/>
       <c r="AG11" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AH11" s="7" t="s">
         <v>6</v>
@@ -8086,15 +8000,14 @@
       <c r="AL11" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="AM11" s="7" t="str">
-        <f>SURTUG!$G$33</f>
-        <v>TANGGAL PULANG</v>
+      <c r="AM11" s="7" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="12" spans="1:39" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E12" s="28"/>
       <c r="G12" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H12" s="7" t="s">
         <v>6</v>
@@ -8104,7 +8017,7 @@
       </c>
       <c r="R12" s="28"/>
       <c r="T12" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="U12" s="7" t="s">
         <v>6</v>
@@ -8114,7 +8027,7 @@
       </c>
       <c r="AE12" s="28"/>
       <c r="AG12" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AH12" s="7" t="s">
         <v>6</v>
@@ -8181,17 +8094,17 @@
     </row>
     <row r="17" spans="1:39" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E17" s="28"/>
       <c r="G17" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H17" s="7" t="s">
         <v>6</v>
@@ -8200,17 +8113,17 @@
         <v>6</v>
       </c>
       <c r="N17" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="O17" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="P17" s="7" t="s">
         <v>6</v>
       </c>
       <c r="R17" s="28"/>
       <c r="T17" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="U17" s="7" t="s">
         <v>6</v>
@@ -8219,17 +8132,17 @@
         <v>6</v>
       </c>
       <c r="AA17" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AB17" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AC17" s="7" t="s">
         <v>6</v>
       </c>
       <c r="AE17" s="28"/>
       <c r="AG17" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AH17" s="7" t="s">
         <v>6</v>
@@ -8240,14 +8153,14 @@
     </row>
     <row r="18" spans="1:39" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E18" s="28"/>
       <c r="G18" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H18" s="7" t="s">
         <v>6</v>
@@ -8256,14 +8169,14 @@
         <v>6</v>
       </c>
       <c r="O18" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P18" s="7" t="s">
         <v>6</v>
       </c>
       <c r="R18" s="28"/>
       <c r="T18" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="U18" s="7" t="s">
         <v>6</v>
@@ -8272,14 +8185,14 @@
         <v>6</v>
       </c>
       <c r="AB18" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AC18" s="7" t="s">
         <v>6</v>
       </c>
       <c r="AE18" s="28"/>
       <c r="AG18" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AH18" s="7" t="s">
         <v>6</v>
@@ -8290,14 +8203,14 @@
     </row>
     <row r="19" spans="1:39" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E19" s="28"/>
       <c r="G19" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H19" s="7" t="s">
         <v>6</v>
@@ -8306,14 +8219,14 @@
         <v>6</v>
       </c>
       <c r="O19" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P19" s="7" t="s">
         <v>6</v>
       </c>
       <c r="R19" s="28"/>
       <c r="T19" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="U19" s="7" t="s">
         <v>6</v>
@@ -8322,14 +8235,14 @@
         <v>6</v>
       </c>
       <c r="AB19" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AC19" s="7" t="s">
         <v>6</v>
       </c>
       <c r="AE19" s="28"/>
       <c r="AG19" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AH19" s="7" t="s">
         <v>6</v>
@@ -8341,7 +8254,7 @@
     <row r="20" spans="1:39" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E20" s="28"/>
       <c r="G20" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H20" s="7" t="s">
         <v>6</v>
@@ -8351,7 +8264,7 @@
       </c>
       <c r="R20" s="28"/>
       <c r="T20" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="U20" s="7" t="s">
         <v>6</v>
@@ -8361,7 +8274,7 @@
       </c>
       <c r="AE20" s="28"/>
       <c r="AG20" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AH20" s="7" t="s">
         <v>6</v>
@@ -8428,10 +8341,10 @@
     </row>
     <row r="25" spans="1:39" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D25" s="31" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F25" s="7" t="s">
         <v>6</v>
@@ -8440,10 +8353,10 @@
         <v>59</v>
       </c>
       <c r="Q25" s="31" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R25" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="S25" s="7" t="s">
         <v>6</v>
@@ -8452,10 +8365,10 @@
         <v>59</v>
       </c>
       <c r="AD25" s="31" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AE25" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AF25" s="7" t="s">
         <v>6</v>
@@ -8466,39 +8379,36 @@
     </row>
     <row r="26" spans="1:39" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E26" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F26" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G26" s="7" t="str">
-        <f>M11</f>
-        <v>TANGGAL PULANG</v>
+      <c r="G26" s="7" t="s">
+        <v>155</v>
       </c>
       <c r="R26" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="S26" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="T26" s="7" t="str">
-        <f>Z11</f>
-        <v>TANGGAL PULANG</v>
+      <c r="T26" s="7" t="s">
+        <v>155</v>
       </c>
       <c r="AE26" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AF26" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="AG26" s="7" t="str">
-        <f>AM11</f>
-        <v>TANGGAL PULANG</v>
+      <c r="AG26" s="7" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="27" spans="1:39" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E27" s="53" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F27" s="53"/>
       <c r="G27" s="53"/>
@@ -8509,7 +8419,7 @@
       <c r="L27" s="53"/>
       <c r="M27" s="53"/>
       <c r="R27" s="53" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="S27" s="53"/>
       <c r="T27" s="53"/>
@@ -8520,7 +8430,7 @@
       <c r="Y27" s="53"/>
       <c r="Z27" s="53"/>
       <c r="AE27" s="53" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AF27" s="53"/>
       <c r="AG27" s="53"/>
@@ -8630,9 +8540,8 @@
       </c>
     </row>
     <row r="35" spans="1:39" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E35" s="27" t="str">
-        <f>SURTUG!$G$50</f>
-        <v>Yayillatul Rochmah, S. Si. Apt</v>
+      <c r="E35" s="27" t="s">
+        <v>160</v>
       </c>
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
@@ -8641,9 +8550,8 @@
       <c r="J35" s="6"/>
       <c r="K35" s="6"/>
       <c r="L35" s="6"/>
-      <c r="R35" s="27" t="str">
-        <f>SURTUG!$G$50</f>
-        <v>Yayillatul Rochmah, S. Si. Apt</v>
+      <c r="R35" s="27" t="s">
+        <v>160</v>
       </c>
       <c r="S35" s="6"/>
       <c r="T35" s="6"/>
@@ -8652,9 +8560,8 @@
       <c r="W35" s="6"/>
       <c r="X35" s="6"/>
       <c r="Y35" s="6"/>
-      <c r="AE35" s="27" t="str">
-        <f>SURTUG!$G$50</f>
-        <v>Yayillatul Rochmah, S. Si. Apt</v>
+      <c r="AE35" s="27" t="s">
+        <v>160</v>
       </c>
       <c r="AF35" s="6"/>
       <c r="AG35" s="6"/>
@@ -8665,9 +8572,8 @@
       <c r="AL35" s="6"/>
     </row>
     <row r="36" spans="1:39" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E36" s="34" t="str">
-        <f>SURTUG!$G$51</f>
-        <v>NIP.19780703 200502 2 006</v>
+      <c r="E36" s="34" t="s">
+        <v>160</v>
       </c>
       <c r="F36" s="6"/>
       <c r="G36" s="6"/>
@@ -8676,9 +8582,8 @@
       <c r="J36" s="6"/>
       <c r="K36" s="6"/>
       <c r="L36" s="6"/>
-      <c r="R36" s="34" t="str">
-        <f>SURTUG!$G$51</f>
-        <v>NIP.19780703 200502 2 006</v>
+      <c r="R36" s="34" t="s">
+        <v>160</v>
       </c>
       <c r="S36" s="6"/>
       <c r="T36" s="6"/>
@@ -8687,9 +8592,8 @@
       <c r="W36" s="6"/>
       <c r="X36" s="6"/>
       <c r="Y36" s="6"/>
-      <c r="AE36" s="34" t="str">
-        <f>SURTUG!$G$51</f>
-        <v>NIP.19780703 200502 2 006</v>
+      <c r="AE36" s="34" t="s">
+        <v>160</v>
       </c>
       <c r="AF36" s="6"/>
       <c r="AG36" s="6"/>
@@ -8724,10 +8628,10 @@
     </row>
     <row r="38" spans="1:39" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="B38" s="35" t="s">
         <v>91</v>
-      </c>
-      <c r="B38" s="35" t="s">
-        <v>92</v>
       </c>
       <c r="C38" s="35"/>
       <c r="D38" s="35"/>
@@ -8741,10 +8645,10 @@
       <c r="L38" s="35"/>
       <c r="M38" s="35"/>
       <c r="N38" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="O38" s="35" t="s">
         <v>91</v>
-      </c>
-      <c r="O38" s="35" t="s">
-        <v>92</v>
       </c>
       <c r="P38" s="35"/>
       <c r="Q38" s="35"/>
@@ -8758,10 +8662,10 @@
       <c r="Y38" s="35"/>
       <c r="Z38" s="35"/>
       <c r="AA38" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="AB38" s="35" t="s">
         <v>91</v>
-      </c>
-      <c r="AB38" s="35" t="s">
-        <v>92</v>
       </c>
       <c r="AC38" s="35"/>
       <c r="AD38" s="35"/>
@@ -8778,60 +8682,57 @@
     <row r="45" spans="1:39" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E45" s="28"/>
       <c r="F45" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G45" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="G45" s="7" t="s">
-        <v>80</v>
-      </c>
       <c r="H45" s="7" t="s">
         <v>6</v>
       </c>
       <c r="L45" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="M45" s="9" t="str">
-        <f>M1</f>
-        <v>NOMOR SPD</v>
+      <c r="M45" s="9" t="s">
+        <v>155</v>
       </c>
       <c r="R45" s="28"/>
       <c r="S45" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="T45" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="T45" s="7" t="s">
-        <v>80</v>
-      </c>
       <c r="U45" s="7" t="s">
         <v>6</v>
       </c>
       <c r="Y45" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="Z45" s="9" t="str">
-        <f>M1</f>
-        <v>NOMOR SPD</v>
+      <c r="Z45" s="9" t="s">
+        <v>155</v>
       </c>
       <c r="AE45" s="28"/>
       <c r="AF45" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="AG45" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="AG45" s="7" t="s">
-        <v>80</v>
-      </c>
       <c r="AH45" s="7" t="s">
         <v>6</v>
       </c>
       <c r="AL45" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="AM45" s="9" t="str">
-        <f>M1</f>
-        <v>NOMOR SPD</v>
+      <c r="AM45" s="9" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="46" spans="1:39" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E46" s="28"/>
       <c r="G46" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H46" s="7" t="s">
         <v>6</v>
@@ -8847,7 +8748,7 @@
       </c>
       <c r="R46" s="28"/>
       <c r="T46" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="U46" s="7" t="s">
         <v>6</v>
@@ -8863,7 +8764,7 @@
       </c>
       <c r="AE46" s="28"/>
       <c r="AG46" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AH46" s="7" t="s">
         <v>6</v>
@@ -8881,21 +8782,21 @@
     <row r="47" spans="1:39" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E47" s="28"/>
       <c r="G47" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="R47" s="28"/>
       <c r="T47" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AE47" s="28"/>
       <c r="AG47" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="48" spans="1:39" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E48" s="28"/>
       <c r="G48" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H48" s="7" t="s">
         <v>6</v>
@@ -8903,13 +8804,12 @@
       <c r="L48" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="M48" s="7" t="str">
-        <f>SURTUG!$G$32</f>
-        <v>TANGGAL BERANGKAT</v>
+      <c r="M48" s="7" t="s">
+        <v>155</v>
       </c>
       <c r="R48" s="28"/>
       <c r="T48" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="U48" s="7" t="s">
         <v>6</v>
@@ -8917,13 +8817,12 @@
       <c r="Y48" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="Z48" s="7" t="str">
-        <f>SURTUG!$G$32</f>
-        <v>TANGGAL BERANGKAT</v>
+      <c r="Z48" s="7" t="s">
+        <v>155</v>
       </c>
       <c r="AE48" s="28"/>
       <c r="AG48" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AH48" s="7" t="s">
         <v>6</v>
@@ -8931,15 +8830,14 @@
       <c r="AL48" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="AM48" s="7" t="str">
-        <f>SURTUG!$G$32</f>
-        <v>TANGGAL BERANGKAT</v>
+      <c r="AM48" s="7" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="49" spans="1:39" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E49" s="28"/>
       <c r="G49" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H49" s="7" t="s">
         <v>6</v>
@@ -8947,13 +8845,12 @@
       <c r="L49" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="M49" s="9" t="str">
-        <f>SURTUG!$G$38</f>
-        <v>NAMA PUSKESMAS</v>
+      <c r="M49" s="9" t="s">
+        <v>155</v>
       </c>
       <c r="R49" s="28"/>
       <c r="T49" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="U49" s="7" t="s">
         <v>6</v>
@@ -8961,13 +8858,12 @@
       <c r="Y49" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="Z49" s="9" t="str">
-        <f>SURTUG!$G$38</f>
-        <v>NAMA PUSKESMAS</v>
+      <c r="Z49" s="9" t="s">
+        <v>155</v>
       </c>
       <c r="AE49" s="28"/>
       <c r="AG49" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AH49" s="7" t="s">
         <v>6</v>
@@ -8975,9 +8871,8 @@
       <c r="AL49" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="AM49" s="9" t="str">
-        <f>SURTUG!$G$38</f>
-        <v>NAMA PUSKESMAS</v>
+      <c r="AM49" s="9" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="50" spans="1:39" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -9033,21 +8928,20 @@
     </row>
     <row r="53" spans="1:39" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B53" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B53" s="7" t="s">
-        <v>86</v>
-      </c>
       <c r="C53" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D53" s="9" t="str">
-        <f>M49</f>
-        <v>NAMA PUSKESMAS</v>
+      <c r="D53" s="9" t="s">
+        <v>155</v>
       </c>
       <c r="E53" s="28"/>
       <c r="G53" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H53" s="7" t="s">
         <v>6</v>
@@ -9055,26 +8949,24 @@
       <c r="L53" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="M53" s="9" t="str">
-        <f>D53</f>
-        <v>NAMA PUSKESMAS</v>
+      <c r="M53" s="9" t="s">
+        <v>155</v>
       </c>
       <c r="N53" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="O53" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="O53" s="7" t="s">
-        <v>86</v>
-      </c>
       <c r="P53" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="Q53" s="9" t="str">
-        <f>Z49</f>
-        <v>NAMA PUSKESMAS</v>
+      <c r="Q53" s="9" t="s">
+        <v>155</v>
       </c>
       <c r="R53" s="28"/>
       <c r="T53" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="U53" s="7" t="s">
         <v>6</v>
@@ -9082,26 +8974,24 @@
       <c r="Y53" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="Z53" s="9" t="str">
-        <f>Q53</f>
-        <v>NAMA PUSKESMAS</v>
+      <c r="Z53" s="9" t="s">
+        <v>155</v>
       </c>
       <c r="AA53" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB53" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="AB53" s="7" t="s">
-        <v>86</v>
-      </c>
       <c r="AC53" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="AD53" s="9" t="str">
-        <f>AM49</f>
-        <v>NAMA PUSKESMAS</v>
+      <c r="AD53" s="9" t="s">
+        <v>155</v>
       </c>
       <c r="AE53" s="28"/>
       <c r="AG53" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AH53" s="7" t="s">
         <v>6</v>
@@ -9109,25 +8999,23 @@
       <c r="AL53" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="AM53" s="9" t="str">
-        <f>AD53</f>
-        <v>NAMA PUSKESMAS</v>
+      <c r="AM53" s="9" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="54" spans="1:39" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B54" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C54" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D54" s="7" t="str">
-        <f>M48</f>
-        <v>TANGGAL BERANGKAT</v>
+      <c r="D54" s="7" t="s">
+        <v>155</v>
       </c>
       <c r="E54" s="28"/>
       <c r="G54" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H54" s="7" t="s">
         <v>6</v>
@@ -9140,18 +9028,17 @@
         <v>Tana Paser</v>
       </c>
       <c r="O54" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P54" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="Q54" s="7" t="str">
-        <f>Z48</f>
-        <v>TANGGAL BERANGKAT</v>
+      <c r="Q54" s="7" t="s">
+        <v>155</v>
       </c>
       <c r="R54" s="28"/>
       <c r="T54" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="U54" s="7" t="s">
         <v>6</v>
@@ -9164,18 +9051,17 @@
         <v>Tana Paser</v>
       </c>
       <c r="AB54" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AC54" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="AD54" s="7" t="str">
-        <f>AM48</f>
-        <v>TANGGAL BERANGKAT</v>
+      <c r="AD54" s="7" t="s">
+        <v>155</v>
       </c>
       <c r="AE54" s="28"/>
       <c r="AG54" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AH54" s="7" t="s">
         <v>6</v>
@@ -9190,14 +9076,14 @@
     </row>
     <row r="55" spans="1:39" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B55" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C55" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E55" s="28"/>
       <c r="G55" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H55" s="7" t="s">
         <v>6</v>
@@ -9205,19 +9091,18 @@
       <c r="L55" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="M55" s="7" t="str">
-        <f>SURTUG!$G$33</f>
-        <v>TANGGAL PULANG</v>
+      <c r="M55" s="7" t="s">
+        <v>155</v>
       </c>
       <c r="O55" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P55" s="7" t="s">
         <v>6</v>
       </c>
       <c r="R55" s="28"/>
       <c r="T55" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="U55" s="7" t="s">
         <v>6</v>
@@ -9225,19 +9110,18 @@
       <c r="Y55" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="Z55" s="7" t="str">
-        <f>SURTUG!$G$33</f>
-        <v>TANGGAL PULANG</v>
+      <c r="Z55" s="7" t="s">
+        <v>155</v>
       </c>
       <c r="AB55" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AC55" s="7" t="s">
         <v>6</v>
       </c>
       <c r="AE55" s="28"/>
       <c r="AG55" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AH55" s="7" t="s">
         <v>6</v>
@@ -9245,15 +9129,14 @@
       <c r="AL55" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="AM55" s="7" t="str">
-        <f>SURTUG!$G$33</f>
-        <v>TANGGAL PULANG</v>
+      <c r="AM55" s="7" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="56" spans="1:39" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E56" s="28"/>
       <c r="G56" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H56" s="7" t="s">
         <v>6</v>
@@ -9263,7 +9146,7 @@
       </c>
       <c r="R56" s="28"/>
       <c r="T56" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="U56" s="7" t="s">
         <v>6</v>
@@ -9273,7 +9156,7 @@
       </c>
       <c r="AE56" s="28"/>
       <c r="AG56" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AH56" s="7" t="s">
         <v>6</v>
@@ -9340,17 +9223,17 @@
     </row>
     <row r="61" spans="1:39" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C61" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E61" s="28"/>
       <c r="G61" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H61" s="7" t="s">
         <v>6</v>
@@ -9359,17 +9242,17 @@
         <v>6</v>
       </c>
       <c r="N61" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="O61" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="P61" s="7" t="s">
         <v>6</v>
       </c>
       <c r="R61" s="28"/>
       <c r="T61" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="U61" s="7" t="s">
         <v>6</v>
@@ -9378,17 +9261,17 @@
         <v>6</v>
       </c>
       <c r="AA61" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AB61" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AC61" s="7" t="s">
         <v>6</v>
       </c>
       <c r="AE61" s="28"/>
       <c r="AG61" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AH61" s="7" t="s">
         <v>6</v>
@@ -9399,14 +9282,14 @@
     </row>
     <row r="62" spans="1:39" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B62" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C62" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E62" s="28"/>
       <c r="G62" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H62" s="7" t="s">
         <v>6</v>
@@ -9415,14 +9298,14 @@
         <v>6</v>
       </c>
       <c r="O62" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P62" s="7" t="s">
         <v>6</v>
       </c>
       <c r="R62" s="28"/>
       <c r="T62" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="U62" s="7" t="s">
         <v>6</v>
@@ -9431,14 +9314,14 @@
         <v>6</v>
       </c>
       <c r="AB62" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AC62" s="7" t="s">
         <v>6</v>
       </c>
       <c r="AE62" s="28"/>
       <c r="AG62" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AH62" s="7" t="s">
         <v>6</v>
@@ -9449,14 +9332,14 @@
     </row>
     <row r="63" spans="1:39" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B63" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C63" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E63" s="28"/>
       <c r="G63" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H63" s="7" t="s">
         <v>6</v>
@@ -9465,14 +9348,14 @@
         <v>6</v>
       </c>
       <c r="O63" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P63" s="7" t="s">
         <v>6</v>
       </c>
       <c r="R63" s="28"/>
       <c r="T63" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="U63" s="7" t="s">
         <v>6</v>
@@ -9481,14 +9364,14 @@
         <v>6</v>
       </c>
       <c r="AB63" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AC63" s="7" t="s">
         <v>6</v>
       </c>
       <c r="AE63" s="28"/>
       <c r="AG63" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AH63" s="7" t="s">
         <v>6</v>
@@ -9500,7 +9383,7 @@
     <row r="64" spans="1:39" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E64" s="28"/>
       <c r="G64" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H64" s="7" t="s">
         <v>6</v>
@@ -9510,7 +9393,7 @@
       </c>
       <c r="R64" s="28"/>
       <c r="T64" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="U64" s="7" t="s">
         <v>6</v>
@@ -9520,7 +9403,7 @@
       </c>
       <c r="AE64" s="28"/>
       <c r="AG64" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AH64" s="7" t="s">
         <v>6</v>
@@ -9587,10 +9470,10 @@
     </row>
     <row r="69" spans="1:39" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D69" s="31" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E69" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F69" s="7" t="s">
         <v>6</v>
@@ -9599,10 +9482,10 @@
         <v>59</v>
       </c>
       <c r="Q69" s="31" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R69" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="S69" s="7" t="s">
         <v>6</v>
@@ -9611,10 +9494,10 @@
         <v>59</v>
       </c>
       <c r="AD69" s="31" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AE69" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AF69" s="7" t="s">
         <v>6</v>
@@ -9625,39 +9508,36 @@
     </row>
     <row r="70" spans="1:39" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E70" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F70" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G70" s="7" t="str">
-        <f>M55</f>
-        <v>TANGGAL PULANG</v>
+      <c r="G70" s="7" t="s">
+        <v>155</v>
       </c>
       <c r="R70" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="S70" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="T70" s="7" t="str">
-        <f>Z55</f>
-        <v>TANGGAL PULANG</v>
+      <c r="T70" s="7" t="s">
+        <v>155</v>
       </c>
       <c r="AE70" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AF70" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="AG70" s="7" t="str">
-        <f>AM55</f>
-        <v>TANGGAL PULANG</v>
+      <c r="AG70" s="7" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="71" spans="1:39" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E71" s="53" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F71" s="53"/>
       <c r="G71" s="53"/>
@@ -9668,7 +9548,7 @@
       <c r="L71" s="53"/>
       <c r="M71" s="53"/>
       <c r="R71" s="53" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="S71" s="53"/>
       <c r="T71" s="53"/>
@@ -9679,7 +9559,7 @@
       <c r="Y71" s="53"/>
       <c r="Z71" s="53"/>
       <c r="AE71" s="53" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AF71" s="53"/>
       <c r="AG71" s="53"/>
@@ -9789,9 +9669,8 @@
       </c>
     </row>
     <row r="79" spans="1:39" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E79" s="27" t="str">
-        <f>SURTUG!$G$50</f>
-        <v>Yayillatul Rochmah, S. Si. Apt</v>
+      <c r="E79" s="27" t="s">
+        <v>160</v>
       </c>
       <c r="F79" s="6"/>
       <c r="G79" s="6"/>
@@ -9800,9 +9679,8 @@
       <c r="J79" s="6"/>
       <c r="K79" s="6"/>
       <c r="L79" s="6"/>
-      <c r="R79" s="27" t="str">
-        <f>SURTUG!$G$50</f>
-        <v>Yayillatul Rochmah, S. Si. Apt</v>
+      <c r="R79" s="27" t="s">
+        <v>160</v>
       </c>
       <c r="S79" s="6"/>
       <c r="T79" s="6"/>
@@ -9811,9 +9689,8 @@
       <c r="W79" s="6"/>
       <c r="X79" s="6"/>
       <c r="Y79" s="6"/>
-      <c r="AE79" s="27" t="str">
-        <f>SURTUG!$G$50</f>
-        <v>Yayillatul Rochmah, S. Si. Apt</v>
+      <c r="AE79" s="27" t="s">
+        <v>160</v>
       </c>
       <c r="AF79" s="6"/>
       <c r="AG79" s="6"/>
@@ -9824,9 +9701,8 @@
       <c r="AL79" s="6"/>
     </row>
     <row r="80" spans="1:39" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E80" s="34" t="str">
-        <f>SURTUG!$G$51</f>
-        <v>NIP.19780703 200502 2 006</v>
+      <c r="E80" s="34" t="s">
+        <v>160</v>
       </c>
       <c r="F80" s="6"/>
       <c r="G80" s="6"/>
@@ -9835,9 +9711,8 @@
       <c r="J80" s="6"/>
       <c r="K80" s="6"/>
       <c r="L80" s="6"/>
-      <c r="R80" s="34" t="str">
-        <f>SURTUG!$G$51</f>
-        <v>NIP.19780703 200502 2 006</v>
+      <c r="R80" s="34" t="s">
+        <v>160</v>
       </c>
       <c r="S80" s="6"/>
       <c r="T80" s="6"/>
@@ -9846,9 +9721,8 @@
       <c r="W80" s="6"/>
       <c r="X80" s="6"/>
       <c r="Y80" s="6"/>
-      <c r="AE80" s="34" t="str">
-        <f>SURTUG!$G$51</f>
-        <v>NIP.19780703 200502 2 006</v>
+      <c r="AE80" s="34" t="s">
+        <v>160</v>
       </c>
       <c r="AF80" s="6"/>
       <c r="AG80" s="6"/>
@@ -9883,10 +9757,10 @@
     </row>
     <row r="82" spans="1:39" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="B82" s="35" t="s">
         <v>91</v>
-      </c>
-      <c r="B82" s="35" t="s">
-        <v>92</v>
       </c>
       <c r="C82" s="35"/>
       <c r="D82" s="35"/>
@@ -9900,10 +9774,10 @@
       <c r="L82" s="35"/>
       <c r="M82" s="35"/>
       <c r="N82" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="O82" s="35" t="s">
         <v>91</v>
-      </c>
-      <c r="O82" s="35" t="s">
-        <v>92</v>
       </c>
       <c r="P82" s="35"/>
       <c r="Q82" s="35"/>
@@ -9917,10 +9791,10 @@
       <c r="Y82" s="35"/>
       <c r="Z82" s="35"/>
       <c r="AA82" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="AB82" s="35" t="s">
         <v>91</v>
-      </c>
-      <c r="AB82" s="35" t="s">
-        <v>92</v>
       </c>
       <c r="AC82" s="35"/>
       <c r="AD82" s="35"/>
@@ -9944,7 +9818,7 @@
     <mergeCell ref="AE71:AM73"/>
   </mergeCells>
   <pageMargins left="0.30381944444444442" right="0.32552083333333331" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="5" orientation="portrait" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="5" orientation="portrait" useFirstPageNumber="1" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -9952,8 +9826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:X56"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25:L26"/>
+    <sheetView view="pageLayout" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T59" sqref="T59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10165,7 +10039,7 @@
     </row>
     <row r="8" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="37" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B8" s="37"/>
       <c r="C8" s="37"/>
@@ -10179,7 +10053,7 @@
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
       <c r="M8" s="37" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N8" s="37"/>
       <c r="O8" s="37"/>
@@ -10221,7 +10095,7 @@
     </row>
     <row r="10" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="38" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B10" s="38"/>
       <c r="C10" s="38"/>
@@ -10230,7 +10104,7 @@
       </c>
       <c r="E10" s="38"/>
       <c r="F10" s="38" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G10" s="38"/>
       <c r="H10" s="38"/>
@@ -10239,7 +10113,7 @@
       <c r="K10" s="38"/>
       <c r="L10" s="38"/>
       <c r="M10" s="38" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N10" s="38"/>
       <c r="O10" s="38"/>
@@ -10248,7 +10122,7 @@
       </c>
       <c r="Q10" s="38"/>
       <c r="R10" s="38" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S10" s="38"/>
       <c r="T10" s="38"/>
@@ -10285,7 +10159,7 @@
     </row>
     <row r="12" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="38" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B12" s="38"/>
       <c r="C12" s="38"/>
@@ -10294,7 +10168,7 @@
       </c>
       <c r="E12" s="38"/>
       <c r="F12" s="38" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G12" s="38"/>
       <c r="H12" s="38"/>
@@ -10303,7 +10177,7 @@
       <c r="K12" s="38"/>
       <c r="L12" s="38"/>
       <c r="M12" s="38" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="N12" s="38"/>
       <c r="O12" s="38"/>
@@ -10312,7 +10186,7 @@
       </c>
       <c r="Q12" s="38"/>
       <c r="R12" s="38" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="S12" s="38"/>
       <c r="T12" s="38"/>
@@ -10357,9 +10231,8 @@
         <v>6</v>
       </c>
       <c r="E14" s="38"/>
-      <c r="F14" s="38" t="str">
-        <f>SURTUG!$G$12</f>
-        <v>TANGGAL BERANGKAT</v>
+      <c r="F14" s="38" t="s">
+        <v>154</v>
       </c>
       <c r="G14" s="38"/>
       <c r="H14" s="38"/>
@@ -10376,9 +10249,8 @@
         <v>6</v>
       </c>
       <c r="Q14" s="38"/>
-      <c r="R14" s="38" t="str">
-        <f>SURTUG!$G$12</f>
-        <v>TANGGAL BERANGKAT</v>
+      <c r="R14" s="38" t="s">
+        <v>154</v>
       </c>
       <c r="S14" s="38"/>
       <c r="T14" s="38"/>
@@ -10423,9 +10295,8 @@
         <v>6</v>
       </c>
       <c r="E16" s="38"/>
-      <c r="F16" s="38" t="str">
-        <f>SURTUG!$G$11</f>
-        <v>NOMOR NOTA DINAS</v>
+      <c r="F16" s="38" t="s">
+        <v>154</v>
       </c>
       <c r="G16" s="38"/>
       <c r="H16" s="38"/>
@@ -10442,9 +10313,8 @@
         <v>6</v>
       </c>
       <c r="Q16" s="38"/>
-      <c r="R16" s="38" t="str">
-        <f>SURTUG!$G$11</f>
-        <v>NOMOR NOTA DINAS</v>
+      <c r="R16" s="38" t="s">
+        <v>154</v>
       </c>
       <c r="S16" s="38"/>
       <c r="T16" s="38"/>
@@ -10481,7 +10351,7 @@
     </row>
     <row r="18" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="38" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B18" s="38"/>
       <c r="C18" s="38"/>
@@ -10490,7 +10360,7 @@
       </c>
       <c r="E18" s="38"/>
       <c r="F18" s="38" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G18" s="38"/>
       <c r="H18" s="38"/>
@@ -10499,7 +10369,7 @@
       <c r="K18" s="38"/>
       <c r="L18" s="38"/>
       <c r="M18" s="38" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="N18" s="38"/>
       <c r="O18" s="38"/>
@@ -10508,7 +10378,7 @@
       </c>
       <c r="Q18" s="38"/>
       <c r="R18" s="38" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="S18" s="38"/>
       <c r="T18" s="38"/>
@@ -10545,7 +10415,7 @@
     </row>
     <row r="20" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="38" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B20" s="38"/>
       <c r="C20" s="38"/>
@@ -10563,7 +10433,7 @@
       <c r="K20" s="38"/>
       <c r="L20" s="38"/>
       <c r="M20" s="38" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N20" s="38"/>
       <c r="O20" s="38"/>
@@ -10609,7 +10479,7 @@
     </row>
     <row r="22" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="38" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B22" s="38"/>
       <c r="C22" s="38"/>
@@ -10618,7 +10488,7 @@
       </c>
       <c r="E22" s="38"/>
       <c r="F22" s="38" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G22" s="38"/>
       <c r="H22" s="38"/>
@@ -10627,7 +10497,7 @@
       <c r="K22" s="38"/>
       <c r="L22" s="38"/>
       <c r="M22" s="38" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N22" s="38"/>
       <c r="O22" s="38"/>
@@ -10636,7 +10506,7 @@
       </c>
       <c r="Q22" s="38"/>
       <c r="R22" s="38" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="S22" s="38"/>
       <c r="T22" s="38"/>
@@ -10699,7 +10569,7 @@
     </row>
     <row r="25" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="38" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B25" s="38"/>
       <c r="C25" s="38"/>
@@ -10718,7 +10588,7 @@
       <c r="K25" s="56"/>
       <c r="L25" s="56"/>
       <c r="M25" s="38" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N25" s="38"/>
       <c r="O25" s="38"/>
@@ -10791,7 +10661,7 @@
     </row>
     <row r="28" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="38" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B28" s="38"/>
       <c r="C28" s="38"/>
@@ -10800,7 +10670,7 @@
       </c>
       <c r="E28" s="38"/>
       <c r="F28" s="57" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G28" s="57"/>
       <c r="H28" s="57"/>
@@ -10809,7 +10679,7 @@
       <c r="K28" s="57"/>
       <c r="L28" s="57"/>
       <c r="M28" s="38" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="N28" s="38"/>
       <c r="O28" s="38"/>
@@ -10818,7 +10688,7 @@
       </c>
       <c r="Q28" s="38"/>
       <c r="R28" s="57" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="S28" s="57"/>
       <c r="T28" s="57"/>
@@ -10907,7 +10777,7 @@
     </row>
     <row r="32" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="38" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B32" s="38"/>
       <c r="C32" s="38"/>
@@ -10917,9 +10787,8 @@
       <c r="E32" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="F32" s="40" t="str">
-        <f>SURTUG!$G$16</f>
-        <v>NAMA1</v>
+      <c r="F32" s="40" t="s">
+        <v>154</v>
       </c>
       <c r="G32" s="38"/>
       <c r="H32" s="38"/>
@@ -10928,7 +10797,7 @@
       <c r="K32" s="38"/>
       <c r="L32" s="38"/>
       <c r="M32" s="38" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="N32" s="38"/>
       <c r="O32" s="38"/>
@@ -10938,9 +10807,8 @@
       <c r="Q32" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="R32" s="40" t="str">
-        <f>SURTUG!$G$16</f>
-        <v>NAMA1</v>
+      <c r="R32" s="40" t="s">
+        <v>154</v>
       </c>
       <c r="S32" s="38"/>
       <c r="T32" s="38"/>
@@ -10955,9 +10823,8 @@
       <c r="C33" s="38"/>
       <c r="D33" s="38"/>
       <c r="E33" s="38"/>
-      <c r="F33" s="38" t="str">
-        <f>SURTUG!$G$18</f>
-        <v>NIP1</v>
+      <c r="F33" s="38" t="s">
+        <v>154</v>
       </c>
       <c r="G33" s="38"/>
       <c r="H33" s="38"/>
@@ -10970,9 +10837,8 @@
       <c r="O33" s="38"/>
       <c r="P33" s="38"/>
       <c r="Q33" s="38"/>
-      <c r="R33" s="38" t="str">
-        <f>SURTUG!$G$18</f>
-        <v>NIP1</v>
+      <c r="R33" s="38" t="s">
+        <v>154</v>
       </c>
       <c r="S33" s="38"/>
       <c r="T33" s="38"/>
@@ -10989,9 +10855,8 @@
       <c r="E34" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="F34" s="40" t="str">
-        <f>SURTUG!$G$21</f>
-        <v>NAMA2</v>
+      <c r="F34" s="40" t="s">
+        <v>154</v>
       </c>
       <c r="G34" s="38"/>
       <c r="H34" s="38"/>
@@ -11006,9 +10871,8 @@
       <c r="Q34" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="R34" s="40" t="str">
-        <f>SURTUG!$G$21</f>
-        <v>NAMA2</v>
+      <c r="R34" s="40" t="s">
+        <v>154</v>
       </c>
       <c r="S34" s="38"/>
       <c r="T34" s="38"/>
@@ -11023,9 +10887,8 @@
       <c r="C35" s="38"/>
       <c r="D35" s="38"/>
       <c r="E35" s="38"/>
-      <c r="F35" s="38" t="str">
-        <f>SURTUG!$G$23</f>
-        <v>NIP2</v>
+      <c r="F35" s="38" t="s">
+        <v>154</v>
       </c>
       <c r="G35" s="38"/>
       <c r="H35" s="38"/>
@@ -11038,9 +10901,8 @@
       <c r="O35" s="38"/>
       <c r="P35" s="38"/>
       <c r="Q35" s="38"/>
-      <c r="R35" s="38" t="str">
-        <f>SURTUG!$G$23</f>
-        <v>NIP2</v>
+      <c r="R35" s="38" t="s">
+        <v>154</v>
       </c>
       <c r="S35" s="38"/>
       <c r="T35" s="38"/>
@@ -11057,9 +10919,8 @@
       <c r="E36" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="F36" s="40" t="str">
-        <f>SURTUG!$G$26</f>
-        <v>NAMA3</v>
+      <c r="F36" s="40" t="s">
+        <v>154</v>
       </c>
       <c r="G36" s="38"/>
       <c r="H36" s="38"/>
@@ -11074,9 +10935,8 @@
       <c r="Q36" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="R36" s="40" t="str">
-        <f>SURTUG!$G$26</f>
-        <v>NAMA3</v>
+      <c r="R36" s="40" t="s">
+        <v>154</v>
       </c>
       <c r="S36" s="38"/>
       <c r="T36" s="38"/>
@@ -11091,9 +10951,8 @@
       <c r="C37" s="38"/>
       <c r="D37" s="38"/>
       <c r="E37" s="38"/>
-      <c r="F37" s="38" t="str">
-        <f>SURTUG!$G$28</f>
-        <v>NIP3</v>
+      <c r="F37" s="38" t="s">
+        <v>154</v>
       </c>
       <c r="G37" s="38"/>
       <c r="H37" s="38"/>
@@ -11106,9 +10965,8 @@
       <c r="O37" s="38"/>
       <c r="P37" s="38"/>
       <c r="Q37" s="38"/>
-      <c r="R37" s="38" t="str">
-        <f>SURTUG!$G$28</f>
-        <v>NIP3</v>
+      <c r="R37" s="38" t="s">
+        <v>154</v>
       </c>
       <c r="S37" s="38"/>
       <c r="T37" s="38"/>
@@ -11145,7 +11003,7 @@
     </row>
     <row r="39" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="38" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B39" s="38"/>
       <c r="C39" s="38"/>
@@ -11153,9 +11011,8 @@
         <v>6</v>
       </c>
       <c r="E39" s="38"/>
-      <c r="F39" s="38" t="str">
-        <f>SURTUG!G31</f>
-        <v>1 (satu) hari</v>
+      <c r="F39" s="38" t="s">
+        <v>154</v>
       </c>
       <c r="G39" s="38"/>
       <c r="H39" s="38"/>
@@ -11164,7 +11021,7 @@
       <c r="K39" s="38"/>
       <c r="L39" s="38"/>
       <c r="M39" s="38" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="N39" s="38"/>
       <c r="O39" s="38"/>
@@ -11174,7 +11031,7 @@
       <c r="Q39" s="38"/>
       <c r="R39" s="38" t="str">
         <f>F39</f>
-        <v>1 (satu) hari</v>
+        <v>z</v>
       </c>
       <c r="S39" s="38"/>
       <c r="T39" s="38"/>
@@ -11211,7 +11068,7 @@
     </row>
     <row r="41" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
@@ -11229,7 +11086,7 @@
       <c r="K41" s="7"/>
       <c r="L41" s="7"/>
       <c r="M41" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="N41" s="7"/>
       <c r="O41" s="7"/>
@@ -11254,13 +11111,13 @@
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="G42" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H42" s="7" t="s">
         <v>109</v>
-      </c>
-      <c r="G42" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="H42" s="7" t="s">
-        <v>110</v>
       </c>
       <c r="I42" s="7"/>
       <c r="J42" s="7"/>
@@ -11272,7 +11129,7 @@
       <c r="P42" s="7"/>
       <c r="Q42" s="7"/>
       <c r="R42" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="S42" s="7" t="s">
         <v>6</v>
@@ -11314,7 +11171,7 @@
     </row>
     <row r="44" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
@@ -11322,9 +11179,8 @@
         <v>6</v>
       </c>
       <c r="E44" s="7"/>
-      <c r="F44" s="41" t="str">
-        <f>SURTUG!G38</f>
-        <v>NAMA PUSKESMAS</v>
+      <c r="F44" s="41" t="s">
+        <v>154</v>
       </c>
       <c r="G44" s="42"/>
       <c r="H44" s="42"/>
@@ -11333,7 +11189,7 @@
       <c r="K44" s="42"/>
       <c r="L44" s="42"/>
       <c r="M44" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N44" s="7"/>
       <c r="O44" s="7"/>
@@ -11343,7 +11199,7 @@
       <c r="Q44" s="7"/>
       <c r="R44" s="41" t="str">
         <f>F44</f>
-        <v>NAMA PUSKESMAS</v>
+        <v>z</v>
       </c>
       <c r="S44" s="41"/>
       <c r="T44" s="41"/>
@@ -11380,7 +11236,7 @@
     </row>
     <row r="46" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="43" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
@@ -11394,7 +11250,7 @@
       <c r="K46" s="6"/>
       <c r="L46" s="6"/>
       <c r="M46" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="N46" s="6"/>
       <c r="O46" s="6"/>
@@ -11495,7 +11351,7 @@
       <c r="F50" s="7"/>
       <c r="G50" s="7"/>
       <c r="H50" s="55" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I50" s="55"/>
       <c r="J50" s="55"/>
@@ -11509,7 +11365,7 @@
       <c r="R50" s="7"/>
       <c r="S50" s="7"/>
       <c r="T50" s="55" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="U50" s="55"/>
       <c r="V50" s="55"/>
@@ -11518,7 +11374,7 @@
     </row>
     <row r="51" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="54" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B51" s="54"/>
       <c r="C51" s="44"/>
@@ -11527,14 +11383,14 @@
       <c r="F51" s="7"/>
       <c r="G51" s="7"/>
       <c r="H51" s="55" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I51" s="55"/>
       <c r="J51" s="55"/>
       <c r="K51" s="55"/>
       <c r="L51" s="55"/>
       <c r="M51" s="54" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N51" s="54"/>
       <c r="O51" s="44"/>
@@ -11543,7 +11399,7 @@
       <c r="R51" s="7"/>
       <c r="S51" s="7"/>
       <c r="T51" s="55" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="U51" s="55"/>
       <c r="V51" s="55"/>
@@ -11637,7 +11493,7 @@
       <c r="F55" s="7"/>
       <c r="G55" s="7"/>
       <c r="H55" s="27" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I55" s="27"/>
       <c r="J55" s="27"/>
@@ -11650,9 +11506,8 @@
       <c r="Q55" s="7"/>
       <c r="R55" s="7"/>
       <c r="S55" s="7"/>
-      <c r="T55" s="27" t="str">
-        <f>H55</f>
-        <v>Agustina Rahmawati, S.A.P</v>
+      <c r="T55" s="27" t="s">
+        <v>160</v>
       </c>
       <c r="U55" s="27"/>
       <c r="V55" s="27"/>
@@ -11668,7 +11523,7 @@
       <c r="F56" s="7"/>
       <c r="G56" s="7"/>
       <c r="H56" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I56" s="6"/>
       <c r="J56" s="6"/>
@@ -11681,9 +11536,8 @@
       <c r="Q56" s="7"/>
       <c r="R56" s="7"/>
       <c r="S56" s="7"/>
-      <c r="T56" s="6" t="str">
-        <f>H56</f>
-        <v>NIP.19800830 200212 2 009</v>
+      <c r="T56" s="6" t="s">
+        <v>160</v>
       </c>
       <c r="U56" s="6"/>
       <c r="V56" s="6"/>
@@ -11704,7 +11558,7 @@
     <mergeCell ref="T50:X50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.32552083333333331" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="5" orientation="portrait" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="5" orientation="portrait" useFirstPageNumber="1" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -11714,7 +11568,7 @@
   <dimension ref="A1:V52"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="R37" sqref="R37"/>
+      <selection activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11921,7 +11775,7 @@
     </row>
     <row r="8" spans="1:22" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="37" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B8" s="37"/>
       <c r="C8" s="37"/>
@@ -11934,7 +11788,7 @@
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="37" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="M8" s="37"/>
       <c r="N8" s="37"/>
@@ -11953,13 +11807,13 @@
       <c r="C9" s="38"/>
       <c r="D9" s="48"/>
       <c r="E9" s="43" t="s">
+        <v>118</v>
+      </c>
+      <c r="F9" s="43" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="38" t="s">
         <v>119</v>
-      </c>
-      <c r="F9" s="43" t="s">
-        <v>6</v>
-      </c>
-      <c r="G9" s="38" t="s">
-        <v>120</v>
       </c>
       <c r="H9" s="43"/>
       <c r="I9" s="43"/>
@@ -11970,14 +11824,13 @@
       <c r="N9" s="38"/>
       <c r="O9" s="48"/>
       <c r="P9" s="43" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="Q9" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="R9" s="38" t="str">
-        <f>G9</f>
-        <v>NOMOR SURAT TUGAS</v>
+      <c r="R9" s="38" t="s">
+        <v>153</v>
       </c>
       <c r="S9" s="43"/>
       <c r="T9" s="43"/>
@@ -12010,41 +11863,40 @@
     </row>
     <row r="11" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="38" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B11" s="38" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="38"/>
       <c r="D11" s="38" t="s">
+        <v>121</v>
+      </c>
+      <c r="E11" s="38" t="s">
+        <v>118</v>
+      </c>
+      <c r="G11" s="38" t="s">
         <v>122</v>
-      </c>
-      <c r="E11" s="38" t="s">
-        <v>119</v>
-      </c>
-      <c r="G11" s="38" t="s">
-        <v>123</v>
       </c>
       <c r="H11" s="38"/>
       <c r="I11" s="38"/>
       <c r="J11" s="38"/>
       <c r="K11" s="38"/>
       <c r="L11" s="38" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="M11" s="38" t="s">
         <v>6</v>
       </c>
       <c r="N11" s="38"/>
       <c r="O11" s="38" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P11" s="38" t="s">
-        <v>119</v>
-      </c>
-      <c r="R11" s="38" t="str">
-        <f>G11</f>
-        <v>NOMOR NOTA DINAS</v>
+        <v>118</v>
+      </c>
+      <c r="R11" s="38" t="s">
+        <v>153</v>
       </c>
       <c r="S11" s="38"/>
       <c r="T11" s="38"/>
@@ -12059,9 +11911,8 @@
         <v>7</v>
       </c>
       <c r="E12" s="38"/>
-      <c r="G12" s="38" t="str">
-        <f>G32</f>
-        <v>TANGGAL BERANGKAT</v>
+      <c r="G12" s="38" t="s">
+        <v>153</v>
       </c>
       <c r="H12" s="38"/>
       <c r="I12" s="38"/>
@@ -12074,9 +11925,8 @@
         <v>7</v>
       </c>
       <c r="P12" s="38"/>
-      <c r="R12" s="38" t="str">
-        <f>G12</f>
-        <v>TANGGAL BERANGKAT</v>
+      <c r="R12" s="38" t="s">
+        <v>153</v>
       </c>
       <c r="S12" s="38"/>
       <c r="T12" s="38"/>
@@ -12109,7 +11959,7 @@
     </row>
     <row r="14" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -12122,7 +11972,7 @@
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
       <c r="L14" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
@@ -12161,7 +12011,7 @@
     </row>
     <row r="16" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="38" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B16" s="38" t="s">
         <v>6</v>
@@ -12177,14 +12027,14 @@
         <v>6</v>
       </c>
       <c r="G16" s="38" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H16" s="38"/>
       <c r="I16" s="38"/>
       <c r="J16" s="38"/>
       <c r="K16" s="38"/>
       <c r="L16" s="38" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M16" s="38" t="s">
         <v>6</v>
@@ -12199,9 +12049,8 @@
       <c r="Q16" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="R16" s="38" t="str">
-        <f>G16</f>
-        <v>NAMA1</v>
+      <c r="R16" s="38" t="s">
+        <v>153</v>
       </c>
       <c r="S16" s="38"/>
       <c r="T16" s="38"/>
@@ -12213,14 +12062,14 @@
       <c r="B17" s="38"/>
       <c r="C17" s="38"/>
       <c r="D17" s="38" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E17" s="38"/>
       <c r="F17" s="38" t="s">
         <v>6</v>
       </c>
       <c r="G17" s="38" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H17" s="38"/>
       <c r="I17" s="38"/>
@@ -12230,15 +12079,14 @@
       <c r="M17" s="38"/>
       <c r="N17" s="38"/>
       <c r="O17" s="38" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="P17" s="38"/>
       <c r="Q17" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="R17" s="38" t="str">
-        <f t="shared" ref="R17:R19" si="0">G17</f>
-        <v>PANGKAT1</v>
+      <c r="R17" s="38" t="s">
+        <v>153</v>
       </c>
       <c r="S17" s="38"/>
       <c r="T17" s="38"/>
@@ -12257,7 +12105,7 @@
         <v>6</v>
       </c>
       <c r="G18" s="38" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H18" s="38"/>
       <c r="I18" s="38"/>
@@ -12273,9 +12121,8 @@
       <c r="Q18" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="R18" s="38" t="str">
-        <f t="shared" si="0"/>
-        <v>NIP1</v>
+      <c r="R18" s="38" t="s">
+        <v>153</v>
       </c>
       <c r="S18" s="38"/>
       <c r="T18" s="38"/>
@@ -12287,14 +12134,14 @@
       <c r="B19" s="38"/>
       <c r="C19" s="38"/>
       <c r="D19" s="38" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E19" s="38"/>
       <c r="F19" s="38" t="s">
         <v>6</v>
       </c>
       <c r="G19" s="38" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H19" s="38"/>
       <c r="I19" s="38"/>
@@ -12304,15 +12151,14 @@
       <c r="M19" s="38"/>
       <c r="N19" s="38"/>
       <c r="O19" s="38" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="P19" s="38"/>
       <c r="Q19" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="R19" s="38" t="str">
-        <f t="shared" si="0"/>
-        <v>JABATAN1</v>
+      <c r="R19" s="38" t="s">
+        <v>153</v>
       </c>
       <c r="S19" s="38"/>
       <c r="T19" s="38"/>
@@ -12357,7 +12203,7 @@
         <v>6</v>
       </c>
       <c r="G21" s="38" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H21" s="38"/>
       <c r="I21" s="38"/>
@@ -12375,9 +12221,8 @@
       <c r="Q21" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="R21" s="38" t="str">
-        <f>G21</f>
-        <v>NAMA2</v>
+      <c r="R21" s="38" t="s">
+        <v>153</v>
       </c>
       <c r="S21" s="38"/>
       <c r="T21" s="38"/>
@@ -12389,14 +12234,14 @@
       <c r="B22" s="38"/>
       <c r="C22" s="38"/>
       <c r="D22" s="38" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E22" s="38"/>
       <c r="F22" s="38" t="s">
         <v>6</v>
       </c>
       <c r="G22" s="38" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H22" s="38"/>
       <c r="I22" s="38"/>
@@ -12406,15 +12251,14 @@
       <c r="M22" s="38"/>
       <c r="N22" s="38"/>
       <c r="O22" s="38" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="P22" s="38"/>
       <c r="Q22" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="R22" s="38" t="str">
-        <f t="shared" ref="R22:R24" si="1">G22</f>
-        <v>PANGKAT2</v>
+      <c r="R22" s="38" t="s">
+        <v>153</v>
       </c>
       <c r="S22" s="38"/>
       <c r="T22" s="38"/>
@@ -12433,7 +12277,7 @@
         <v>6</v>
       </c>
       <c r="G23" s="38" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H23" s="38"/>
       <c r="I23" s="38"/>
@@ -12449,9 +12293,8 @@
       <c r="Q23" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="R23" s="38" t="str">
-        <f t="shared" si="1"/>
-        <v>NIP2</v>
+      <c r="R23" s="38" t="s">
+        <v>153</v>
       </c>
       <c r="S23" s="38"/>
       <c r="T23" s="38"/>
@@ -12463,14 +12306,14 @@
       <c r="B24" s="38"/>
       <c r="C24" s="38"/>
       <c r="D24" s="38" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E24" s="38"/>
       <c r="F24" s="38" t="s">
         <v>6</v>
       </c>
       <c r="G24" s="38" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H24" s="38"/>
       <c r="I24" s="38"/>
@@ -12480,15 +12323,14 @@
       <c r="M24" s="38"/>
       <c r="N24" s="38"/>
       <c r="O24" s="38" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="P24" s="38"/>
       <c r="Q24" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="R24" s="38" t="str">
-        <f t="shared" si="1"/>
-        <v>JABATAN2</v>
+      <c r="R24" s="38" t="s">
+        <v>153</v>
       </c>
       <c r="S24" s="38"/>
       <c r="T24" s="38"/>
@@ -12533,7 +12375,7 @@
         <v>6</v>
       </c>
       <c r="G26" s="38" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H26" s="38"/>
       <c r="I26" s="38"/>
@@ -12551,9 +12393,8 @@
       <c r="Q26" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="R26" s="38" t="str">
-        <f>G26</f>
-        <v>NAMA3</v>
+      <c r="R26" s="38" t="s">
+        <v>153</v>
       </c>
       <c r="S26" s="38"/>
       <c r="T26" s="38"/>
@@ -12565,14 +12406,14 @@
       <c r="B27" s="38"/>
       <c r="C27" s="38"/>
       <c r="D27" s="38" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E27" s="38"/>
       <c r="F27" s="38" t="s">
         <v>6</v>
       </c>
       <c r="G27" s="38" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H27" s="38"/>
       <c r="I27" s="38"/>
@@ -12582,15 +12423,14 @@
       <c r="M27" s="38"/>
       <c r="N27" s="38"/>
       <c r="O27" s="38" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="P27" s="38"/>
       <c r="Q27" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="R27" s="38" t="str">
-        <f t="shared" ref="R27:R29" si="2">G27</f>
-        <v>PANGKAT3</v>
+      <c r="R27" s="38" t="s">
+        <v>153</v>
       </c>
       <c r="S27" s="38"/>
       <c r="T27" s="38"/>
@@ -12609,7 +12449,7 @@
         <v>6</v>
       </c>
       <c r="G28" s="38" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H28" s="38"/>
       <c r="I28" s="38"/>
@@ -12625,9 +12465,8 @@
       <c r="Q28" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="R28" s="38" t="str">
-        <f t="shared" si="2"/>
-        <v>NIP3</v>
+      <c r="R28" s="38" t="s">
+        <v>153</v>
       </c>
       <c r="S28" s="38"/>
       <c r="T28" s="38"/>
@@ -12639,14 +12478,14 @@
       <c r="B29" s="38"/>
       <c r="C29" s="38"/>
       <c r="D29" s="38" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E29" s="38"/>
       <c r="F29" s="38" t="s">
         <v>6</v>
       </c>
       <c r="G29" s="38" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H29" s="38"/>
       <c r="I29" s="38"/>
@@ -12656,15 +12495,14 @@
       <c r="M29" s="38"/>
       <c r="N29" s="38"/>
       <c r="O29" s="38" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="P29" s="38"/>
       <c r="Q29" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="R29" s="38" t="str">
-        <f t="shared" si="2"/>
-        <v>JABATAN3</v>
+      <c r="R29" s="38" t="s">
+        <v>153</v>
       </c>
       <c r="S29" s="38"/>
       <c r="T29" s="38"/>
@@ -12697,7 +12535,7 @@
     </row>
     <row r="31" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="59" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B31" s="59"/>
       <c r="C31" s="59"/>
@@ -12715,7 +12553,7 @@
       <c r="J31" s="38"/>
       <c r="K31" s="38"/>
       <c r="L31" s="59" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="M31" s="59"/>
       <c r="N31" s="59"/>
@@ -12724,9 +12562,8 @@
       <c r="Q31" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="R31" s="38" t="str">
-        <f>G31</f>
-        <v>1 (satu) hari</v>
+      <c r="R31" s="38" t="s">
+        <v>153</v>
       </c>
       <c r="S31" s="38"/>
       <c r="T31" s="38"/>
@@ -12735,7 +12572,7 @@
     </row>
     <row r="32" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="59" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B32" s="59"/>
       <c r="C32" s="59"/>
@@ -12745,14 +12582,14 @@
         <v>6</v>
       </c>
       <c r="G32" s="38" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H32" s="38"/>
       <c r="I32" s="38"/>
       <c r="J32" s="38"/>
       <c r="K32" s="38"/>
       <c r="L32" s="59" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M32" s="59"/>
       <c r="N32" s="59"/>
@@ -12761,9 +12598,8 @@
       <c r="Q32" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="R32" s="38" t="str">
-        <f>G32</f>
-        <v>TANGGAL BERANGKAT</v>
+      <c r="R32" s="38" t="s">
+        <v>153</v>
       </c>
       <c r="S32" s="38"/>
       <c r="T32" s="38"/>
@@ -12772,7 +12608,7 @@
     </row>
     <row r="33" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="59" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B33" s="59"/>
       <c r="C33" s="59"/>
@@ -12782,14 +12618,14 @@
         <v>6</v>
       </c>
       <c r="G33" s="38" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H33" s="38"/>
       <c r="I33" s="38"/>
       <c r="J33" s="38"/>
       <c r="K33" s="38"/>
       <c r="L33" s="59" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="M33" s="59"/>
       <c r="N33" s="59"/>
@@ -12798,9 +12634,8 @@
       <c r="Q33" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="R33" s="38" t="str">
-        <f t="shared" ref="R33" si="3">G33</f>
-        <v>TANGGAL PULANG</v>
+      <c r="R33" s="38" t="s">
+        <v>153</v>
       </c>
       <c r="S33" s="38"/>
       <c r="T33" s="38"/>
@@ -12833,7 +12668,7 @@
     </row>
     <row r="35" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="38" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B35" s="38"/>
       <c r="C35" s="38"/>
@@ -12843,14 +12678,14 @@
         <v>6</v>
       </c>
       <c r="G35" s="56" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H35" s="56"/>
       <c r="I35" s="56"/>
       <c r="J35" s="56"/>
       <c r="K35" s="56"/>
       <c r="L35" s="38" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="M35" s="38"/>
       <c r="N35" s="38"/>
@@ -12918,7 +12753,7 @@
     </row>
     <row r="38" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="38" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B38" s="38"/>
       <c r="C38" s="38"/>
@@ -12928,14 +12763,14 @@
         <v>6</v>
       </c>
       <c r="G38" s="38" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H38" s="38"/>
       <c r="I38" s="38"/>
       <c r="J38" s="38"/>
       <c r="K38" s="38"/>
       <c r="L38" s="38" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="M38" s="38"/>
       <c r="N38" s="38"/>
@@ -12944,9 +12779,8 @@
       <c r="Q38" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="R38" s="38" t="str">
-        <f>G38</f>
-        <v>NAMA PUSKESMAS</v>
+      <c r="R38" s="38" t="s">
+        <v>153</v>
       </c>
       <c r="S38" s="38"/>
       <c r="T38" s="38"/>
@@ -13009,7 +12843,7 @@
       <c r="E41" s="38"/>
       <c r="F41" s="38"/>
       <c r="G41" s="38" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H41" s="38"/>
       <c r="I41" s="38" t="s">
@@ -13026,7 +12860,7 @@
       <c r="P41" s="38"/>
       <c r="Q41" s="38"/>
       <c r="R41" s="38" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="S41" s="38"/>
       <c r="T41" s="38" t="s">
@@ -13045,15 +12879,14 @@
       <c r="E42" s="38"/>
       <c r="F42" s="38"/>
       <c r="G42" s="38" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H42" s="38"/>
       <c r="I42" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="J42" s="38" t="str">
-        <f>G32</f>
-        <v>TANGGAL BERANGKAT</v>
+      <c r="J42" s="38" t="s">
+        <v>153</v>
       </c>
       <c r="K42" s="38"/>
       <c r="L42" s="38"/>
@@ -13063,15 +12896,14 @@
       <c r="P42" s="38"/>
       <c r="Q42" s="38"/>
       <c r="R42" s="38" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="S42" s="38"/>
       <c r="T42" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="U42" s="38" t="str">
-        <f>J42</f>
-        <v>TANGGAL BERANGKAT</v>
+      <c r="U42" s="38" t="s">
+        <v>153</v>
       </c>
       <c r="V42" s="38"/>
     </row>
@@ -13131,7 +12963,7 @@
       <c r="E45" s="38"/>
       <c r="F45" s="38"/>
       <c r="G45" s="58" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H45" s="58"/>
       <c r="I45" s="58"/>
@@ -13144,7 +12976,7 @@
       <c r="P45" s="38"/>
       <c r="Q45" s="38"/>
       <c r="R45" s="58" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="S45" s="58"/>
       <c r="T45" s="58"/>
@@ -13159,7 +12991,7 @@
       <c r="E46" s="38"/>
       <c r="F46" s="38"/>
       <c r="G46" s="58" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H46" s="58"/>
       <c r="I46" s="58"/>
@@ -13172,7 +13004,7 @@
       <c r="P46" s="38"/>
       <c r="Q46" s="38"/>
       <c r="R46" s="58" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="S46" s="58"/>
       <c r="T46" s="58"/>
@@ -13181,15 +13013,14 @@
     </row>
     <row r="50" spans="7:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G50" s="16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H50" s="4"/>
       <c r="I50" s="4"/>
       <c r="J50" s="4"/>
       <c r="K50" s="4"/>
-      <c r="R50" s="16" t="str">
-        <f>G50</f>
-        <v>Yayillatul Rochmah, S. Si. Apt</v>
+      <c r="R50" s="16" t="s">
+        <v>160</v>
       </c>
       <c r="S50" s="4"/>
       <c r="T50" s="4"/>
@@ -13198,15 +13029,14 @@
     </row>
     <row r="51" spans="7:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G51" s="43" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H51" s="4"/>
       <c r="I51" s="4"/>
       <c r="J51" s="4"/>
       <c r="K51" s="4"/>
-      <c r="R51" s="43" t="str">
-        <f>G51</f>
-        <v>NIP.19780703 200502 2 006</v>
+      <c r="R51" s="43" t="s">
+        <v>160</v>
       </c>
       <c r="S51" s="4"/>
       <c r="T51" s="4"/>
@@ -13239,7 +13069,7 @@
     <mergeCell ref="R46:V46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.64583333333333337" top="0.3125" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="5" orientation="portrait" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="5" orientation="portrait" useFirstPageNumber="1" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>